<commit_message>
Added more unseen data
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96AF998-C98A-BB4D-99FB-652E393FB54E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C18568C-FDBF-B34C-A145-292731D04823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34920" yWindow="-2240" windowWidth="32160" windowHeight="18340" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9111,7 +9111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G868"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A838" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A840" zoomScale="75" workbookViewId="0">
       <selection activeCell="I788" sqref="I788"/>
     </sheetView>
   </sheetViews>
@@ -36562,8 +36562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9983360C-B04E-264E-A2FD-A3AF9B5DD60B}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T81"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
This is the knownlenses excel
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D89EF8-DB1C-2749-8BBF-9DCEE6BE7CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8084E7-4FC3-8440-ABA2-A7F22027AB83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9111,7 +9111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G868"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A735" zoomScale="75" workbookViewId="0">
       <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
@@ -28450,8 +28450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F87BBA-BC16-DD40-96FA-DA2C592E0EA9}">
   <dimension ref="A1:K229"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B229"/>
+    <sheetView topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T224" sqref="T224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed unseen known lenses ra and dec
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC377D8-3535-3C47-A0F5-4CA044D452A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259D8E88-8249-D84C-A6DB-62F88DB80B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="-1440" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9111,8 +9111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A854" workbookViewId="0">
-      <selection activeCell="G883" sqref="G883"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A807" sqref="A807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26854,7 +26854,7 @@
         <v>2763</v>
       </c>
       <c r="B803" s="3">
-        <v>167.57370833333334</v>
+        <v>167.573708333333</v>
       </c>
       <c r="C803" s="3">
         <f t="shared" si="30"/>

</xml_diff>

<commit_message>
Printing confusion matrix as well as the predicted lenses in text files
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5309D4-FA6C-3743-A355-A4D3E6F99301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC64A41B-A7FE-A64D-9FB3-E7714668C796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="-1440" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9153,8 +9153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A724" workbookViewId="0">
-      <selection activeCell="A752" sqref="A752"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -59477,8 +59477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31C520D-257B-3141-B803-1F468B25B845}">
   <dimension ref="A1:O186"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132:C186"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed KerasCnn.py removing data augmentation
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC64A41B-A7FE-A64D-9FB3-E7714668C796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BA52A4-4FB8-CB46-908A-F5C08525C52B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="-1440" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9153,8 +9153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Not sure why I have to keep commiting the unseen table
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BA52A4-4FB8-CB46-908A-F5C08525C52B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94C838-BC0C-8F4A-818B-6193209473D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="-1440" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -9153,7 +9153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A550" workbookViewId="0">
       <selection activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying to get y and x labels on graph
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94C838-BC0C-8F4A-818B-6193209473D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581810A2-2E7E-6843-BC23-A75A3D66B874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33660" yWindow="-1440" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
+    <workbookView xWindow="50640" yWindow="-2180" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lenses" sheetId="1" r:id="rId1"/>
@@ -8797,7 +8797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8831,12 +8831,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9153,8 +9157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A550" workbookViewId="0">
-      <selection activeCell="A262" sqref="A262"/>
+    <sheetView tabSelected="1" topLeftCell="A726" workbookViewId="0">
+      <selection activeCell="G736" sqref="G736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21204,7 +21208,7 @@
         <f t="shared" ref="C544:C572" si="22">IF(D544&lt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="D544">
+      <c r="D544" s="3">
         <v>-9.2541916666666673</v>
       </c>
       <c r="E544" s="4">
@@ -21226,7 +21230,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D545">
+      <c r="D545" s="3">
         <v>-11.153244444444445</v>
       </c>
       <c r="E545" s="4">
@@ -21248,7 +21252,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D546">
+      <c r="D546" s="3">
         <v>-6.5822555555555553</v>
       </c>
       <c r="E546" s="4">
@@ -21270,7 +21274,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D547">
+      <c r="D547" s="3">
         <v>-8.3539583333333329</v>
       </c>
       <c r="E547" s="4">
@@ -21292,7 +21296,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D548">
+      <c r="D548" s="3">
         <v>-10.785541666666667</v>
       </c>
       <c r="E548" s="4">
@@ -21314,7 +21318,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D549">
+      <c r="D549" s="3">
         <v>-7.5807722222222216</v>
       </c>
       <c r="E549" s="4">
@@ -21336,7 +21340,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D550">
+      <c r="D550" s="3">
         <v>-9.714863888888889</v>
       </c>
       <c r="E550" s="4">
@@ -21358,7 +21362,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D551">
+      <c r="D551" s="3">
         <v>-10.400688888888888</v>
       </c>
       <c r="E551" s="4">
@@ -21380,7 +21384,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D552">
+      <c r="D552" s="3">
         <v>-11.096286111111112</v>
       </c>
       <c r="E552" s="4">
@@ -21402,7 +21406,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D553">
+      <c r="D553" s="3">
         <v>-6.950369444444445</v>
       </c>
       <c r="E553" s="4">
@@ -21424,7 +21428,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D554">
+      <c r="D554" s="3">
         <v>-7.4160583333333339</v>
       </c>
       <c r="E554" s="4">
@@ -21446,7 +21450,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D555">
+      <c r="D555" s="3">
         <v>-9.6146361111111105</v>
       </c>
       <c r="E555" s="4">
@@ -21468,7 +21472,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D556">
+      <c r="D556" s="3">
         <v>-7.0244638888888886</v>
       </c>
       <c r="E556" s="4">
@@ -21490,7 +21494,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D557">
+      <c r="D557" s="3">
         <v>-6.7197944444444442</v>
       </c>
       <c r="E557" s="4">
@@ -21512,7 +21516,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D558">
+      <c r="D558" s="3">
         <v>-3.9158555555555554</v>
       </c>
       <c r="E558" s="4">
@@ -21534,7 +21538,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D559">
+      <c r="D559" s="3">
         <v>-4.7782194444444448</v>
       </c>
       <c r="E559" s="4">
@@ -21556,7 +21560,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D560">
+      <c r="D560" s="3">
         <v>-3.8812888888888888</v>
       </c>
       <c r="E560" s="4">
@@ -21578,7 +21582,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D561">
+      <c r="D561" s="3">
         <v>-10.203849999999999</v>
       </c>
       <c r="E561" s="4">
@@ -21600,7 +21604,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D562">
+      <c r="D562" s="3">
         <v>-4.4581111111111111</v>
       </c>
       <c r="E562" s="4">
@@ -21622,7 +21626,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D563">
+      <c r="D563" s="3">
         <v>-9.6455833333333327</v>
       </c>
       <c r="E563" s="4">
@@ -21644,7 +21648,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D564">
+      <c r="D564" s="3">
         <v>-7.7318944444444444</v>
       </c>
       <c r="E564" s="4">
@@ -21666,7 +21670,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D565">
+      <c r="D565" s="3">
         <v>-5.5923305555555549</v>
       </c>
       <c r="E565" s="4">
@@ -21688,7 +21692,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D566">
+      <c r="D566" s="3">
         <v>-4.0840861111111106</v>
       </c>
       <c r="E566" s="4">
@@ -21710,7 +21714,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D567">
+      <c r="D567" s="3">
         <v>-7.6065444444444443</v>
       </c>
       <c r="E567" s="4">
@@ -21732,7 +21736,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D568">
+      <c r="D568" s="3">
         <v>-7.350366666666666</v>
       </c>
       <c r="E568" s="4">
@@ -21754,7 +21758,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D569">
+      <c r="D569" s="3">
         <v>-9.5851805555555565</v>
       </c>
       <c r="E569" s="4">
@@ -21776,7 +21780,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D570">
+      <c r="D570" s="3">
         <v>-9.9608583333333325</v>
       </c>
       <c r="E570" s="4">
@@ -21798,7 +21802,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D571">
+      <c r="D571" s="3">
         <v>-7.5325361111111109</v>
       </c>
       <c r="E571" s="4">
@@ -21820,7 +21824,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="D572">
+      <c r="D572" s="3">
         <v>-9.3046500000000005</v>
       </c>
       <c r="E572" s="4">
@@ -21842,7 +21846,7 @@
         <f t="shared" ref="C573:C636" si="23">IF(D573&lt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="D573">
+      <c r="D573" s="3">
         <v>-7.0566111111111107</v>
       </c>
       <c r="E573" s="4">
@@ -21864,7 +21868,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D574">
+      <c r="D574" s="3">
         <v>-10.263972222222222</v>
       </c>
       <c r="E574" s="4">
@@ -21886,7 +21890,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D575">
+      <c r="D575" s="3">
         <v>-10.555536111111111</v>
       </c>
       <c r="E575" s="4">
@@ -21908,7 +21912,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D576">
+      <c r="D576" s="3">
         <v>-5.2600444444444445</v>
       </c>
       <c r="E576" s="4">
@@ -21930,7 +21934,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D577">
+      <c r="D577" s="3">
         <v>-10.100638888888888</v>
       </c>
       <c r="E577" s="4">
@@ -21952,7 +21956,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D578">
+      <c r="D578" s="3">
         <v>-4.0286999999999997</v>
       </c>
       <c r="E578" s="4">
@@ -21974,7 +21978,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D579">
+      <c r="D579" s="3">
         <v>-5.4664472222222225</v>
       </c>
       <c r="E579" s="4">
@@ -21996,7 +22000,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D580">
+      <c r="D580" s="3">
         <v>-10.871236111111111</v>
       </c>
       <c r="E580" s="4">
@@ -22018,7 +22022,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D581">
+      <c r="D581" s="3">
         <v>-7.7199194444444448</v>
       </c>
       <c r="E581" s="4">
@@ -22040,7 +22044,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D582">
+      <c r="D582" s="3">
         <v>-6.7924055555555558</v>
       </c>
       <c r="E582" s="4">
@@ -22062,7 +22066,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D583">
+      <c r="D583" s="3">
         <v>-6.4851111111111113</v>
       </c>
       <c r="E583" s="4">
@@ -22084,7 +22088,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D584">
+      <c r="D584" s="3">
         <v>-10.980127777777778</v>
       </c>
       <c r="E584" s="4">
@@ -22106,7 +22110,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D585">
+      <c r="D585" s="3">
         <v>-3.7738416666666668</v>
       </c>
       <c r="E585" s="4">
@@ -22128,7 +22132,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D586">
+      <c r="D586" s="3">
         <v>-4.785277777777778</v>
       </c>
       <c r="E586" s="4">
@@ -22150,7 +22154,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D587">
+      <c r="D587" s="3">
         <v>-4.1930611111111116</v>
       </c>
       <c r="E587" s="4">
@@ -22172,7 +22176,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D588">
+      <c r="D588" s="3">
         <v>-4.0327388888888889</v>
       </c>
       <c r="E588" s="4">
@@ -22194,7 +22198,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D589">
+      <c r="D589" s="3">
         <v>-4.012544444444444</v>
       </c>
       <c r="E589" s="4">
@@ -22216,7 +22220,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D590">
+      <c r="D590" s="3">
         <v>-4.0177138888888893</v>
       </c>
       <c r="E590" s="4">
@@ -22238,7 +22242,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D591">
+      <c r="D591" s="3">
         <v>-4.9093166666666672</v>
       </c>
       <c r="E591" s="4">
@@ -22260,7 +22264,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D592">
+      <c r="D592" s="3">
         <v>-4.0556555555555551</v>
       </c>
       <c r="E592" s="4">
@@ -22282,7 +22286,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D593">
+      <c r="D593" s="3">
         <v>-7.6273666666666671</v>
       </c>
       <c r="E593" s="4">
@@ -22304,7 +22308,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D594">
+      <c r="D594" s="3">
         <v>-4.4572944444444449</v>
       </c>
       <c r="E594" s="4">
@@ -22326,7 +22330,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D595">
+      <c r="D595" s="3">
         <v>-7.8222749999999994</v>
       </c>
       <c r="E595" s="4">
@@ -22348,7 +22352,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D596">
+      <c r="D596" s="3">
         <v>-9.1249611111111122</v>
       </c>
       <c r="E596" s="4">
@@ -22370,7 +22374,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D597">
+      <c r="D597" s="3">
         <v>-9.8292888888888879</v>
       </c>
       <c r="E597" s="4">
@@ -22392,7 +22396,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D598">
+      <c r="D598" s="3">
         <v>-5.9015388888888891</v>
       </c>
       <c r="E598" s="4">
@@ -22414,7 +22418,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D599">
+      <c r="D599" s="3">
         <v>-3.8411277777777779</v>
       </c>
       <c r="E599" s="4">
@@ -22436,7 +22440,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D600">
+      <c r="D600" s="3">
         <v>-5.9179527777777778</v>
       </c>
       <c r="E600" s="4">
@@ -22458,7 +22462,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D601">
+      <c r="D601" s="3">
         <v>-8.8439916666666676</v>
       </c>
       <c r="E601" s="4">
@@ -22480,7 +22484,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D602">
+      <c r="D602" s="3">
         <v>-4.6439472222222218</v>
       </c>
       <c r="E602" s="4">
@@ -22502,7 +22506,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D603">
+      <c r="D603" s="3">
         <v>-9.9757666666666669</v>
       </c>
       <c r="E603" s="4">
@@ -22524,7 +22528,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D604">
+      <c r="D604" s="3">
         <v>-4.1209138888888885</v>
       </c>
       <c r="E604" s="4">
@@ -22546,7 +22550,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D605">
+      <c r="D605" s="3">
         <v>-1.3981388888888888</v>
       </c>
       <c r="E605" s="4">
@@ -22568,7 +22572,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D606">
+      <c r="D606" s="3">
         <v>-3.7211888888888889</v>
       </c>
       <c r="E606" s="4">
@@ -22590,7 +22594,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D607">
+      <c r="D607" s="3">
         <v>-4.0912111111111109</v>
       </c>
       <c r="E607" s="4">
@@ -22612,7 +22616,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D608">
+      <c r="D608" s="3">
         <v>-3.2480861111111112</v>
       </c>
       <c r="E608" s="4">
@@ -22634,7 +22638,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D609">
+      <c r="D609" s="3">
         <v>-1.3603000000000001</v>
       </c>
       <c r="E609" s="4">
@@ -22656,7 +22660,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D610">
+      <c r="D610" s="3">
         <v>-4.154933333333334</v>
       </c>
       <c r="E610" s="4">
@@ -22678,7 +22682,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D611">
+      <c r="D611" s="3">
         <v>-2.7074000000000003</v>
       </c>
       <c r="E611" s="4">
@@ -22700,7 +22704,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D612">
+      <c r="D612" s="3">
         <v>-1.0201527777777777</v>
       </c>
       <c r="E612" s="4">
@@ -22722,7 +22726,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D613">
+      <c r="D613" s="3">
         <v>-1.2168694444444446</v>
       </c>
       <c r="E613" s="4">
@@ -22744,7 +22748,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D614">
+      <c r="D614" s="3">
         <v>-2.6571638888888889</v>
       </c>
       <c r="E614" s="4">
@@ -22766,7 +22770,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D615">
+      <c r="D615" s="3">
         <v>-3.7541250000000002</v>
       </c>
       <c r="E615" s="4">
@@ -22788,7 +22792,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D616">
+      <c r="D616" s="3">
         <v>-1.5370527777777776</v>
       </c>
       <c r="E616" s="4">
@@ -22810,7 +22814,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D617">
+      <c r="D617" s="3">
         <v>-2.5150416666666668</v>
       </c>
       <c r="E617" s="4">
@@ -22832,7 +22836,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D618">
+      <c r="D618" s="3">
         <v>-2.515911111111111</v>
       </c>
       <c r="E618" s="4">
@@ -22854,7 +22858,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D619">
+      <c r="D619" s="3">
         <v>-0.99801388888888887</v>
       </c>
       <c r="E619" s="4">
@@ -22876,7 +22880,7 @@
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="D620">
+      <c r="D620" s="3">
         <v>-2.0549166666666663</v>
       </c>
       <c r="E620" s="4">
@@ -22898,7 +22902,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D621">
+      <c r="D621" s="3">
         <v>2.5122166666666668</v>
       </c>
       <c r="E621" s="4">
@@ -22920,7 +22924,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D622">
+      <c r="D622" s="3">
         <v>2.4989166666666667</v>
       </c>
       <c r="E622" s="4">
@@ -22942,7 +22946,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D623">
+      <c r="D623" s="3">
         <v>2.3171638888888886</v>
       </c>
       <c r="E623" s="4">
@@ -22964,7 +22968,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D624">
+      <c r="D624" s="3">
         <v>2.3598194444444447</v>
       </c>
       <c r="E624" s="4">
@@ -22986,7 +22990,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D625">
+      <c r="D625" s="3">
         <v>2.3684861111111113</v>
       </c>
       <c r="E625" s="4">
@@ -23008,7 +23012,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D626">
+      <c r="D626" s="3">
         <v>2.1942944444444441</v>
       </c>
       <c r="E626" s="4">
@@ -23030,7 +23034,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D627">
+      <c r="D627" s="3">
         <v>2.498677777777778</v>
       </c>
       <c r="E627" s="4">
@@ -23052,7 +23056,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D628">
+      <c r="D628" s="3">
         <v>2.6267972222222222</v>
       </c>
       <c r="E628" s="4">
@@ -23074,7 +23078,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D629">
+      <c r="D629" s="3">
         <v>55.45194444444445</v>
       </c>
       <c r="E629" s="4">
@@ -23096,7 +23100,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D630">
+      <c r="D630" s="3">
         <v>53.295544444444445</v>
       </c>
       <c r="E630" s="4">
@@ -23118,7 +23122,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D631">
+      <c r="D631" s="3">
         <v>55.593769444444447</v>
       </c>
       <c r="E631" s="4">
@@ -23140,7 +23144,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D632">
+      <c r="D632" s="3">
         <v>56.130391666666668</v>
       </c>
       <c r="E632" s="4">
@@ -23162,7 +23166,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D633">
+      <c r="D633" s="3">
         <v>56.905697222222223</v>
       </c>
       <c r="E633" s="4">
@@ -23184,7 +23188,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D634">
+      <c r="D634" s="3">
         <v>53.036005555555555</v>
       </c>
       <c r="E634" s="4">
@@ -23206,7 +23210,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D635">
+      <c r="D635" s="3">
         <v>55.746327777777779</v>
       </c>
       <c r="E635" s="4">
@@ -23228,7 +23232,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D636">
+      <c r="D636" s="3">
         <v>57.14778888888889</v>
       </c>
       <c r="E636" s="4">
@@ -23250,7 +23254,7 @@
         <f t="shared" ref="C637:C700" si="25">IF(D637&lt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="D637">
+      <c r="D637" s="3">
         <v>57.397336111111109</v>
       </c>
       <c r="E637" s="4">
@@ -23272,7 +23276,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D638">
+      <c r="D638" s="3">
         <v>52.006861111111114</v>
       </c>
       <c r="E638" s="4">
@@ -23294,7 +23298,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D639">
+      <c r="D639" s="3">
         <v>54.763522222222221</v>
       </c>
       <c r="E639" s="4">
@@ -23316,7 +23320,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D640">
+      <c r="D640" s="3">
         <v>54.485588888888891</v>
       </c>
       <c r="E640" s="4">
@@ -23338,7 +23342,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D641">
+      <c r="D641" s="3">
         <v>52.202752777777782</v>
       </c>
       <c r="E641" s="4">
@@ -23360,7 +23364,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D642">
+      <c r="D642" s="3">
         <v>53.729088888888889</v>
       </c>
       <c r="E642" s="4">
@@ -23382,7 +23386,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D643">
+      <c r="D643" s="3">
         <v>54.784330555555556</v>
       </c>
       <c r="E643" s="4">
@@ -23404,7 +23408,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D644">
+      <c r="D644" s="3">
         <v>56.70449444444445</v>
       </c>
       <c r="E644" s="4">
@@ -23426,7 +23430,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D645">
+      <c r="D645" s="3">
         <v>53.436511111111109</v>
       </c>
       <c r="E645" s="4">
@@ -23448,7 +23452,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D646">
+      <c r="D646" s="3">
         <v>51.291286111111113</v>
       </c>
       <c r="E646" s="4">
@@ -23470,7 +23474,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D647">
+      <c r="D647" s="3">
         <v>52.495141666666669</v>
       </c>
       <c r="E647" s="4">
@@ -23492,7 +23496,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D648">
+      <c r="D648" s="3">
         <v>52.839547222222222</v>
       </c>
       <c r="E648" s="4">
@@ -23514,7 +23518,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D649">
+      <c r="D649" s="3">
         <v>51.41097222222222</v>
       </c>
       <c r="E649" s="4">
@@ -23536,7 +23540,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D650">
+      <c r="D650" s="3">
         <v>57.442749999999997</v>
       </c>
       <c r="E650" s="4">
@@ -23558,7 +23562,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D651">
+      <c r="D651" s="3">
         <v>57.123463888888892</v>
       </c>
       <c r="E651" s="4">
@@ -23580,7 +23584,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D652">
+      <c r="D652" s="3">
         <v>57.756638888888887</v>
       </c>
       <c r="E652" s="4">
@@ -23602,7 +23606,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D653">
+      <c r="D653" s="3">
         <v>56.66343333333333</v>
       </c>
       <c r="E653" s="4">
@@ -23624,7 +23628,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D654">
+      <c r="D654" s="3">
         <v>52.218455555555558</v>
       </c>
       <c r="E654" s="4">
@@ -23646,7 +23650,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D655">
+      <c r="D655" s="3">
         <v>55.779991666666668</v>
       </c>
       <c r="E655" s="4">
@@ -23668,7 +23672,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D656">
+      <c r="D656" s="3">
         <v>55.556336111111108</v>
       </c>
       <c r="E656" s="4">
@@ -23690,7 +23694,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D657">
+      <c r="D657" s="3">
         <v>57.476869444444446</v>
       </c>
       <c r="E657" s="4">
@@ -23712,7 +23716,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D658">
+      <c r="D658" s="3">
         <v>51.360019444444447</v>
       </c>
       <c r="E658" s="4">
@@ -23734,7 +23738,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D659">
+      <c r="D659" s="3">
         <v>56.988936111111109</v>
       </c>
       <c r="E659" s="4">
@@ -23756,7 +23760,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D660">
+      <c r="D660" s="3">
         <v>4.1690055555555556</v>
       </c>
       <c r="E660" s="4">
@@ -23778,7 +23782,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D661">
+      <c r="D661" s="3">
         <v>1.7859916666666666</v>
       </c>
       <c r="E661" s="4">
@@ -23800,7 +23804,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D662">
+      <c r="D662" s="3">
         <v>2.0885805555555557</v>
       </c>
       <c r="E662" s="4">
@@ -23822,7 +23826,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D663">
+      <c r="D663" s="3">
         <v>1.7843638888888889</v>
       </c>
       <c r="E663" s="4">
@@ -23844,7 +23848,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D664">
+      <c r="D664" s="3">
         <v>4.191902777777778</v>
       </c>
       <c r="E664" s="4">
@@ -23866,7 +23870,7 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="D665">
+      <c r="D665" s="3">
         <v>-0.5102916666666667</v>
       </c>
       <c r="E665" s="4">
@@ -23888,7 +23892,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D666">
+      <c r="D666" s="3">
         <v>0.81003888888888897</v>
       </c>
       <c r="E666" s="4">
@@ -23910,7 +23914,7 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="D667" s="24">
+      <c r="D667" s="25">
         <v>-17.515619444444443</v>
       </c>
       <c r="E667" s="4">
@@ -23932,7 +23936,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="D668">
+      <c r="D668" s="3">
         <v>1.1760694444444446</v>
       </c>
       <c r="E668" s="4">
@@ -23954,7 +23958,7 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="D669">
+      <c r="D669" s="3">
         <v>-0.64349999999999996</v>
       </c>
       <c r="E669" s="4">
@@ -23976,7 +23980,7 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="D670">
+      <c r="D670" s="3">
         <v>-0.88413611111111112</v>
       </c>
       <c r="E670" s="4">
@@ -25462,7 +25466,7 @@
       </c>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A738" s="12" t="s">
+      <c r="A738" s="28" t="s">
         <v>2850</v>
       </c>
       <c r="B738" s="3">
@@ -25484,7 +25488,7 @@
       </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A739" s="12" t="s">
+      <c r="A739" s="28" t="s">
         <v>2851</v>
       </c>
       <c r="B739" s="3">
@@ -25506,7 +25510,7 @@
       </c>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A740" s="12" t="s">
+      <c r="A740" s="28" t="s">
         <v>2852</v>
       </c>
       <c r="B740" s="3">
@@ -25528,7 +25532,7 @@
       </c>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A741" s="12" t="s">
+      <c r="A741" s="28" t="s">
         <v>2853</v>
       </c>
       <c r="B741" s="3">
@@ -25550,7 +25554,7 @@
       </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A742" s="12" t="s">
+      <c r="A742" s="28" t="s">
         <v>2854</v>
       </c>
       <c r="B742" s="3">
@@ -25572,7 +25576,7 @@
       </c>
     </row>
     <row r="743" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A743" s="12" t="s">
+      <c r="A743" s="28" t="s">
         <v>2855</v>
       </c>
       <c r="B743" s="3">
@@ -25594,7 +25598,7 @@
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A744" s="12" t="s">
+      <c r="A744" s="28" t="s">
         <v>2856</v>
       </c>
       <c r="B744" s="3">
@@ -25616,7 +25620,7 @@
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A745" s="14" t="s">
+      <c r="A745" s="28" t="s">
         <v>2857</v>
       </c>
       <c r="B745" s="3">
@@ -25638,7 +25642,7 @@
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A746" s="14" t="s">
+      <c r="A746" s="28" t="s">
         <v>2858</v>
       </c>
       <c r="B746" s="3">
@@ -25660,7 +25664,7 @@
       </c>
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A747" s="14" t="s">
+      <c r="A747" s="28" t="s">
         <v>2859</v>
       </c>
       <c r="B747" s="3">
@@ -25682,7 +25686,7 @@
       </c>
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A748" s="14" t="s">
+      <c r="A748" s="28" t="s">
         <v>2860</v>
       </c>
       <c r="B748" s="3">
@@ -25704,7 +25708,7 @@
       </c>
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A749" s="14" t="s">
+      <c r="A749" s="28" t="s">
         <v>2861</v>
       </c>
       <c r="B749" s="3">
@@ -25726,7 +25730,7 @@
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A750" s="14" t="s">
+      <c r="A750" s="28" t="s">
         <v>2862</v>
       </c>
       <c r="B750" s="3">
@@ -25748,7 +25752,7 @@
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A751" s="14" t="s">
+      <c r="A751" s="28" t="s">
         <v>2863</v>
       </c>
       <c r="B751" s="3">
@@ -25770,7 +25774,7 @@
       </c>
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A752" s="2" t="s">
+      <c r="A752" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B752" s="3">
@@ -25792,7 +25796,7 @@
       </c>
     </row>
     <row r="753" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A753" s="2" t="s">
+      <c r="A753" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B753" s="3">
@@ -25814,7 +25818,7 @@
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A754" s="2" t="s">
+      <c r="A754" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B754" s="3">
@@ -25836,7 +25840,7 @@
       </c>
     </row>
     <row r="755" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A755" s="2" t="s">
+      <c r="A755" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B755" s="3">
@@ -25858,7 +25862,7 @@
       </c>
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A756" s="2" t="s">
+      <c r="A756" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B756" s="3">
@@ -25880,7 +25884,7 @@
       </c>
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A757" s="2" t="s">
+      <c r="A757" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B757" s="3">
@@ -25902,7 +25906,7 @@
       </c>
     </row>
     <row r="758" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A758" s="2" t="s">
+      <c r="A758" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B758" s="3">
@@ -25924,7 +25928,7 @@
       </c>
     </row>
     <row r="759" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A759" s="2" t="s">
+      <c r="A759" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B759" s="3">
@@ -25946,7 +25950,7 @@
       </c>
     </row>
     <row r="760" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A760" s="2" t="s">
+      <c r="A760" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B760" s="3">
@@ -25968,7 +25972,7 @@
       </c>
     </row>
     <row r="761" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A761" s="2" t="s">
+      <c r="A761" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B761" s="3">
@@ -25990,7 +25994,7 @@
       </c>
     </row>
     <row r="762" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A762" s="2" t="s">
+      <c r="A762" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B762" s="3">
@@ -26012,7 +26016,7 @@
       </c>
     </row>
     <row r="763" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A763" s="2" t="s">
+      <c r="A763" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B763" s="3">
@@ -26034,7 +26038,7 @@
       </c>
     </row>
     <row r="764" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A764" s="2" t="s">
+      <c r="A764" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B764" s="3">
@@ -26056,7 +26060,7 @@
       </c>
     </row>
     <row r="765" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A765" s="2" t="s">
+      <c r="A765" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B765" s="3">
@@ -26078,7 +26082,7 @@
       </c>
     </row>
     <row r="766" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A766" s="2" t="s">
+      <c r="A766" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B766" s="3">
@@ -26100,7 +26104,7 @@
       </c>
     </row>
     <row r="767" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A767" s="2" t="s">
+      <c r="A767" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B767" s="3">
@@ -26122,7 +26126,7 @@
       </c>
     </row>
     <row r="768" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A768" s="2" t="s">
+      <c r="A768" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B768" s="3">
@@ -26144,7 +26148,7 @@
       </c>
     </row>
     <row r="769" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A769" s="2" t="s">
+      <c r="A769" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B769" s="3">
@@ -26166,7 +26170,7 @@
       </c>
     </row>
     <row r="770" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A770" s="2" t="s">
+      <c r="A770" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B770" s="3">
@@ -26188,7 +26192,7 @@
       </c>
     </row>
     <row r="771" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A771" s="2" t="s">
+      <c r="A771" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B771" s="3">
@@ -26210,7 +26214,7 @@
       </c>
     </row>
     <row r="772" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A772" s="2" t="s">
+      <c r="A772" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B772" s="3">
@@ -26232,7 +26236,7 @@
       </c>
     </row>
     <row r="773" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A773" s="2" t="s">
+      <c r="A773" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B773" s="3">
@@ -26254,7 +26258,7 @@
       </c>
     </row>
     <row r="774" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A774" s="2" t="s">
+      <c r="A774" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B774" s="3">
@@ -26276,7 +26280,7 @@
       </c>
     </row>
     <row r="775" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A775" s="2" t="s">
+      <c r="A775" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B775" s="3">
@@ -26298,7 +26302,7 @@
       </c>
     </row>
     <row r="776" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A776" s="2" t="s">
+      <c r="A776" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B776" s="3">
@@ -26320,7 +26324,7 @@
       </c>
     </row>
     <row r="777" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A777" s="2" t="s">
+      <c r="A777" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B777" s="3">
@@ -26342,7 +26346,7 @@
       </c>
     </row>
     <row r="778" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A778" s="2" t="s">
+      <c r="A778" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B778" s="3">
@@ -26364,7 +26368,7 @@
       </c>
     </row>
     <row r="779" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A779" s="2" t="s">
+      <c r="A779" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B779" s="3">
@@ -26386,7 +26390,7 @@
       </c>
     </row>
     <row r="780" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A780" s="2" t="s">
+      <c r="A780" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B780" s="3">
@@ -26408,7 +26412,7 @@
       </c>
     </row>
     <row r="781" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A781" s="2" t="s">
+      <c r="A781" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B781" s="3">
@@ -26430,7 +26434,7 @@
       </c>
     </row>
     <row r="782" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A782" s="2" t="s">
+      <c r="A782" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B782" s="3">
@@ -26452,7 +26456,7 @@
       </c>
     </row>
     <row r="783" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A783" s="2" t="s">
+      <c r="A783" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B783" s="3">
@@ -26474,7 +26478,7 @@
       </c>
     </row>
     <row r="784" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A784" s="2" t="s">
+      <c r="A784" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B784" s="3">
@@ -26496,7 +26500,7 @@
       </c>
     </row>
     <row r="785" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A785" s="2" t="s">
+      <c r="A785" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B785" s="3">
@@ -26518,7 +26522,7 @@
       </c>
     </row>
     <row r="786" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A786" s="2" t="s">
+      <c r="A786" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B786" s="3">
@@ -26540,7 +26544,7 @@
       </c>
     </row>
     <row r="787" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A787" s="2" t="s">
+      <c r="A787" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B787" s="3">
@@ -26562,7 +26566,7 @@
       </c>
     </row>
     <row r="788" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A788" s="2" t="s">
+      <c r="A788" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B788" s="3">
@@ -26584,7 +26588,7 @@
       </c>
     </row>
     <row r="789" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A789" s="2" t="s">
+      <c r="A789" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B789" s="3">
@@ -26606,7 +26610,7 @@
       </c>
     </row>
     <row r="790" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A790" s="2" t="s">
+      <c r="A790" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B790" s="3">
@@ -26628,7 +26632,7 @@
       </c>
     </row>
     <row r="791" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A791" s="2" t="s">
+      <c r="A791" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B791" s="3">
@@ -26650,7 +26654,7 @@
       </c>
     </row>
     <row r="792" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A792" s="2" t="s">
+      <c r="A792" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B792" s="3">
@@ -26672,7 +26676,7 @@
       </c>
     </row>
     <row r="793" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A793" s="2" t="s">
+      <c r="A793" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B793" s="3">
@@ -26694,7 +26698,7 @@
       </c>
     </row>
     <row r="794" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A794" s="2" t="s">
+      <c r="A794" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B794" s="3">
@@ -26716,7 +26720,7 @@
       </c>
     </row>
     <row r="795" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A795" s="2" t="s">
+      <c r="A795" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B795" s="3">
@@ -26738,7 +26742,7 @@
       </c>
     </row>
     <row r="796" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A796" s="2" t="s">
+      <c r="A796" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B796" s="3">
@@ -26760,7 +26764,7 @@
       </c>
     </row>
     <row r="797" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A797" s="2" t="s">
+      <c r="A797" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B797" s="3">
@@ -26782,7 +26786,7 @@
       </c>
     </row>
     <row r="798" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A798" s="2" t="s">
+      <c r="A798" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B798" s="3">
@@ -26804,7 +26808,7 @@
       </c>
     </row>
     <row r="799" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A799" s="2" t="s">
+      <c r="A799" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B799" s="3">
@@ -26826,7 +26830,7 @@
       </c>
     </row>
     <row r="800" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A800" s="2" t="s">
+      <c r="A800" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B800" s="3">
@@ -26848,7 +26852,7 @@
       </c>
     </row>
     <row r="801" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A801" s="2" t="s">
+      <c r="A801" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B801" s="3">
@@ -26870,7 +26874,7 @@
       </c>
     </row>
     <row r="802" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A802" s="2" t="s">
+      <c r="A802" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B802" s="3">
@@ -26892,7 +26896,7 @@
       </c>
     </row>
     <row r="803" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A803" s="2" t="s">
+      <c r="A803" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B803" s="3">
@@ -26914,7 +26918,7 @@
       </c>
     </row>
     <row r="804" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A804" s="2" t="s">
+      <c r="A804" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B804" s="3">
@@ -26936,7 +26940,7 @@
       </c>
     </row>
     <row r="805" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A805" s="2" t="s">
+      <c r="A805" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B805" s="3">
@@ -26958,7 +26962,7 @@
       </c>
     </row>
     <row r="806" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A806" s="2" t="s">
+      <c r="A806" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B806" s="3">
@@ -26980,7 +26984,7 @@
       </c>
     </row>
     <row r="807" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A807" s="2" t="s">
+      <c r="A807" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B807" s="3">
@@ -27002,7 +27006,7 @@
       </c>
     </row>
     <row r="808" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A808" s="2" t="s">
+      <c r="A808" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B808" s="3">
@@ -27024,7 +27028,7 @@
       </c>
     </row>
     <row r="809" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A809" s="2" t="s">
+      <c r="A809" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B809" s="3">
@@ -27046,7 +27050,7 @@
       </c>
     </row>
     <row r="810" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A810" s="2" t="s">
+      <c r="A810" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B810" s="3">
@@ -27068,7 +27072,7 @@
       </c>
     </row>
     <row r="811" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A811" s="2" t="s">
+      <c r="A811" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B811" s="3">
@@ -27090,7 +27094,7 @@
       </c>
     </row>
     <row r="812" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A812" s="2" t="s">
+      <c r="A812" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B812" s="3">
@@ -27112,7 +27116,7 @@
       </c>
     </row>
     <row r="813" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A813" s="2" t="s">
+      <c r="A813" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B813" s="3">
@@ -27134,7 +27138,7 @@
       </c>
     </row>
     <row r="814" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A814" s="2" t="s">
+      <c r="A814" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B814" s="3">
@@ -27156,7 +27160,7 @@
       </c>
     </row>
     <row r="815" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A815" s="2" t="s">
+      <c r="A815" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B815" s="3">
@@ -27178,7 +27182,7 @@
       </c>
     </row>
     <row r="816" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A816" s="2" t="s">
+      <c r="A816" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B816" s="3">
@@ -27200,7 +27204,7 @@
       </c>
     </row>
     <row r="817" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A817" s="2" t="s">
+      <c r="A817" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B817" s="3">
@@ -27222,7 +27226,7 @@
       </c>
     </row>
     <row r="818" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A818" s="2" t="s">
+      <c r="A818" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B818" s="3">
@@ -27244,7 +27248,7 @@
       </c>
     </row>
     <row r="819" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A819" s="2" t="s">
+      <c r="A819" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B819" s="3">
@@ -27266,7 +27270,7 @@
       </c>
     </row>
     <row r="820" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A820" s="2" t="s">
+      <c r="A820" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B820" s="3">
@@ -27288,7 +27292,7 @@
       </c>
     </row>
     <row r="821" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A821" s="2" t="s">
+      <c r="A821" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B821" s="3">
@@ -27310,7 +27314,7 @@
       </c>
     </row>
     <row r="822" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A822" s="2" t="s">
+      <c r="A822" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B822" s="3">
@@ -27332,7 +27336,7 @@
       </c>
     </row>
     <row r="823" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A823" s="2" t="s">
+      <c r="A823" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B823" s="3">
@@ -27354,7 +27358,7 @@
       </c>
     </row>
     <row r="824" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A824" s="2" t="s">
+      <c r="A824" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B824" s="3">
@@ -27376,7 +27380,7 @@
       </c>
     </row>
     <row r="825" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A825" s="2" t="s">
+      <c r="A825" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B825" s="3">
@@ -27398,7 +27402,7 @@
       </c>
     </row>
     <row r="826" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A826" s="2" t="s">
+      <c r="A826" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B826" s="3">
@@ -27420,7 +27424,7 @@
       </c>
     </row>
     <row r="827" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A827" s="2" t="s">
+      <c r="A827" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B827" s="3">
@@ -27442,7 +27446,7 @@
       </c>
     </row>
     <row r="828" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A828" s="2" t="s">
+      <c r="A828" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B828" s="3">
@@ -27464,7 +27468,7 @@
       </c>
     </row>
     <row r="829" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A829" s="2" t="s">
+      <c r="A829" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B829" s="3">
@@ -27486,7 +27490,7 @@
       </c>
     </row>
     <row r="830" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A830" s="2" t="s">
+      <c r="A830" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B830" s="3">
@@ -27508,7 +27512,7 @@
       </c>
     </row>
     <row r="831" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A831" s="2" t="s">
+      <c r="A831" s="3" t="s">
         <v>2763</v>
       </c>
       <c r="B831" s="3">
@@ -27530,7 +27534,7 @@
       </c>
     </row>
     <row r="832" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A832" t="s">
+      <c r="A832" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B832" s="3">
@@ -27552,7 +27556,7 @@
       </c>
     </row>
     <row r="833" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A833" t="s">
+      <c r="A833" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B833" s="3">
@@ -27574,7 +27578,7 @@
       </c>
     </row>
     <row r="834" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A834" t="s">
+      <c r="A834" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B834" s="3">
@@ -27596,7 +27600,7 @@
       </c>
     </row>
     <row r="835" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A835" t="s">
+      <c r="A835" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B835" s="3">
@@ -27618,7 +27622,7 @@
       </c>
     </row>
     <row r="836" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A836" t="s">
+      <c r="A836" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B836" s="3">
@@ -27640,7 +27644,7 @@
       </c>
     </row>
     <row r="837" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A837" t="s">
+      <c r="A837" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B837" s="3">
@@ -27662,7 +27666,7 @@
       </c>
     </row>
     <row r="838" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A838" t="s">
+      <c r="A838" s="3" t="s">
         <v>166</v>
       </c>
       <c r="B838" s="3">
@@ -27684,7 +27688,7 @@
       </c>
     </row>
     <row r="839" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A839" t="s">
+      <c r="A839" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B839" s="3">
@@ -27706,7 +27710,7 @@
       </c>
     </row>
     <row r="840" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A840" t="s">
+      <c r="A840" s="3" t="s">
         <v>168</v>
       </c>
       <c r="B840" s="3">
@@ -27728,7 +27732,7 @@
       </c>
     </row>
     <row r="841" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A841" t="s">
+      <c r="A841" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B841" s="3">
@@ -27750,7 +27754,7 @@
       </c>
     </row>
     <row r="842" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A842" t="s">
+      <c r="A842" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B842" s="3">
@@ -27772,7 +27776,7 @@
       </c>
     </row>
     <row r="843" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A843" t="s">
+      <c r="A843" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B843" s="3">
@@ -27794,7 +27798,7 @@
       </c>
     </row>
     <row r="844" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A844" t="s">
+      <c r="A844" s="3" t="s">
         <v>172</v>
       </c>
       <c r="B844" s="3">
@@ -27816,7 +27820,7 @@
       </c>
     </row>
     <row r="845" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A845" t="s">
+      <c r="A845" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B845" s="3">
@@ -27838,7 +27842,7 @@
       </c>
     </row>
     <row r="846" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A846" t="s">
+      <c r="A846" s="3" t="s">
         <v>174</v>
       </c>
       <c r="B846" s="3">
@@ -27860,7 +27864,7 @@
       </c>
     </row>
     <row r="847" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A847" t="s">
+      <c r="A847" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B847" s="3">
@@ -27882,7 +27886,7 @@
       </c>
     </row>
     <row r="848" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A848" t="s">
+      <c r="A848" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B848" s="3">
@@ -27904,7 +27908,7 @@
       </c>
     </row>
     <row r="849" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A849" t="s">
+      <c r="A849" s="3" t="s">
         <v>177</v>
       </c>
       <c r="B849" s="3">
@@ -27926,7 +27930,7 @@
       </c>
     </row>
     <row r="850" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A850" t="s">
+      <c r="A850" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B850" s="3">
@@ -27948,7 +27952,7 @@
       </c>
     </row>
     <row r="851" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A851" t="s">
+      <c r="A851" s="3" t="s">
         <v>179</v>
       </c>
       <c r="B851" s="3">
@@ -27970,7 +27974,7 @@
       </c>
     </row>
     <row r="852" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A852" t="s">
+      <c r="A852" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B852" s="3">
@@ -27992,7 +27996,7 @@
       </c>
     </row>
     <row r="853" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A853" t="s">
+      <c r="A853" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B853" s="3">
@@ -28014,7 +28018,7 @@
       </c>
     </row>
     <row r="854" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A854" t="s">
+      <c r="A854" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B854" s="3">
@@ -28036,7 +28040,7 @@
       </c>
     </row>
     <row r="855" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A855" t="s">
+      <c r="A855" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B855" s="3">
@@ -28058,7 +28062,7 @@
       </c>
     </row>
     <row r="856" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A856" t="s">
+      <c r="A856" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B856" s="3">
@@ -28080,7 +28084,7 @@
       </c>
     </row>
     <row r="857" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A857" t="s">
+      <c r="A857" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B857" s="3">
@@ -28102,7 +28106,7 @@
       </c>
     </row>
     <row r="858" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A858" t="s">
+      <c r="A858" s="3" t="s">
         <v>186</v>
       </c>
       <c r="B858" s="3">
@@ -28124,7 +28128,7 @@
       </c>
     </row>
     <row r="859" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A859" t="s">
+      <c r="A859" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B859" s="3">
@@ -28146,7 +28150,7 @@
       </c>
     </row>
     <row r="860" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A860" t="s">
+      <c r="A860" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B860" s="3">
@@ -28168,7 +28172,7 @@
       </c>
     </row>
     <row r="861" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A861" t="s">
+      <c r="A861" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B861" s="3">
@@ -28190,7 +28194,7 @@
       </c>
     </row>
     <row r="862" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A862" t="s">
+      <c r="A862" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B862" s="3">
@@ -28212,7 +28216,7 @@
       </c>
     </row>
     <row r="863" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A863" t="s">
+      <c r="A863" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B863" s="3">
@@ -28234,7 +28238,7 @@
       </c>
     </row>
     <row r="864" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A864" t="s">
+      <c r="A864" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B864" s="3">
@@ -28256,7 +28260,7 @@
       </c>
     </row>
     <row r="865" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A865" t="s">
+      <c r="A865" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B865" s="3">
@@ -28278,7 +28282,7 @@
       </c>
     </row>
     <row r="866" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A866" t="s">
+      <c r="A866" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B866" s="3">
@@ -28300,7 +28304,7 @@
       </c>
     </row>
     <row r="867" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A867" t="s">
+      <c r="A867" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B867" s="3">
@@ -28322,7 +28326,7 @@
       </c>
     </row>
     <row r="868" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A868" t="s">
+      <c r="A868" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B868" s="3">
@@ -28344,7 +28348,7 @@
       </c>
     </row>
     <row r="869" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A869" t="s">
+      <c r="A869" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B869" s="3">
@@ -28366,7 +28370,7 @@
       </c>
     </row>
     <row r="870" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A870" t="s">
+      <c r="A870" s="3" t="s">
         <v>198</v>
       </c>
       <c r="B870" s="3">
@@ -28388,7 +28392,7 @@
       </c>
     </row>
     <row r="871" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A871" t="s">
+      <c r="A871" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B871" s="3">
@@ -28410,7 +28414,7 @@
       </c>
     </row>
     <row r="872" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A872" t="s">
+      <c r="A872" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B872" s="3">
@@ -28432,7 +28436,7 @@
       </c>
     </row>
     <row r="873" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A873" t="s">
+      <c r="A873" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B873" s="3">
@@ -28454,7 +28458,7 @@
       </c>
     </row>
     <row r="874" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A874" t="s">
+      <c r="A874" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B874" s="3">
@@ -28476,7 +28480,7 @@
       </c>
     </row>
     <row r="875" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A875" t="s">
+      <c r="A875" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B875" s="3">
@@ -28498,7 +28502,7 @@
       </c>
     </row>
     <row r="876" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A876" t="s">
+      <c r="A876" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B876" s="3">
@@ -28520,7 +28524,7 @@
       </c>
     </row>
     <row r="877" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A877" t="s">
+      <c r="A877" s="3" t="s">
         <v>205</v>
       </c>
       <c r="B877" s="3">
@@ -28542,7 +28546,7 @@
       </c>
     </row>
     <row r="878" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A878" t="s">
+      <c r="A878" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B878" s="3">
@@ -28564,7 +28568,7 @@
       </c>
     </row>
     <row r="879" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A879" t="s">
+      <c r="A879" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B879" s="3">
@@ -28586,7 +28590,7 @@
       </c>
     </row>
     <row r="880" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A880" t="s">
+      <c r="A880" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B880" s="3">
@@ -28608,7 +28612,7 @@
       </c>
     </row>
     <row r="881" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A881" t="s">
+      <c r="A881" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B881" s="3">
@@ -28630,7 +28634,7 @@
       </c>
     </row>
     <row r="882" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A882" t="s">
+      <c r="A882" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B882" s="3">
@@ -41113,16 +41117,16 @@
       <c r="A1" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
         <v>1108</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" t="s">
         <v>2357</v>
       </c>
@@ -52018,16 +52022,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -64678,10 +64682,10 @@
       <c r="F1" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="27" t="s">
         <v>719</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
Adding things we have tried to the folder
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581810A2-2E7E-6843-BC23-A75A3D66B874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33A3185-E31E-2F4F-9018-87801DFBBB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50640" yWindow="-2180" windowWidth="28800" windowHeight="17540" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lenses" sheetId="1" r:id="rId1"/>
-    <sheet name="St13" sheetId="11" r:id="rId2"/>
-    <sheet name="M12" sheetId="10" r:id="rId3"/>
-    <sheet name="F08" sheetId="9" r:id="rId4"/>
-    <sheet name="D17" sheetId="2" r:id="rId5"/>
-    <sheet name="S18" sheetId="3" r:id="rId6"/>
-    <sheet name="W18" sheetId="4" r:id="rId7"/>
-    <sheet name="J19" sheetId="5" r:id="rId8"/>
-    <sheet name="J19a" sheetId="6" r:id="rId9"/>
-    <sheet name="H20a" sheetId="7" r:id="rId10"/>
-    <sheet name="Jae20" sheetId="8" r:id="rId11"/>
+    <sheet name="Predicted Lenses" sheetId="12" r:id="rId2"/>
+    <sheet name="St13" sheetId="11" r:id="rId3"/>
+    <sheet name="M12" sheetId="10" r:id="rId4"/>
+    <sheet name="F08" sheetId="9" r:id="rId5"/>
+    <sheet name="D17" sheetId="2" r:id="rId6"/>
+    <sheet name="S18" sheetId="3" r:id="rId7"/>
+    <sheet name="W18" sheetId="4" r:id="rId8"/>
+    <sheet name="J19" sheetId="5" r:id="rId9"/>
+    <sheet name="J19a" sheetId="6" r:id="rId10"/>
+    <sheet name="H20a" sheetId="7" r:id="rId11"/>
+    <sheet name="Jae20" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8257" uniqueCount="2864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8328" uniqueCount="2895">
   <si>
     <t>PAPER_TILE</t>
   </si>
@@ -8635,14 +8636,109 @@
   </si>
   <si>
     <t>J182434686</t>
+  </si>
+  <si>
+    <t>Referenced in</t>
+  </si>
+  <si>
+    <t>DES TILE</t>
+  </si>
+  <si>
+    <t>DES0158-0416</t>
+  </si>
+  <si>
+    <t>DES0035-5123</t>
+  </si>
+  <si>
+    <t>DES2242+0209</t>
+  </si>
+  <si>
+    <t>DES0239-0124</t>
+  </si>
+  <si>
+    <t>DES0100-0707</t>
+  </si>
+  <si>
+    <t>DES2305+0209</t>
+  </si>
+  <si>
+    <t>DES0312-3623</t>
+  </si>
+  <si>
+    <t>DES0011-4623</t>
+  </si>
+  <si>
+    <t>DES0212-0750</t>
+  </si>
+  <si>
+    <t>DES0212-0333</t>
+  </si>
+  <si>
+    <t>DES2234+0001</t>
+  </si>
+  <si>
+    <t>DES0000+0209</t>
+  </si>
+  <si>
+    <t>DES0232-0333</t>
+  </si>
+  <si>
+    <t>DES0023-4914</t>
+  </si>
+  <si>
+    <t>DES0020-5040</t>
+  </si>
+  <si>
+    <t>DES0216-1041</t>
+  </si>
+  <si>
+    <t>DES2214+0126</t>
+  </si>
+  <si>
+    <t>DES0006-4206</t>
+  </si>
+  <si>
+    <t>DES0025-4123</t>
+  </si>
+  <si>
+    <t>39.926</t>
+  </si>
+  <si>
+    <t>48.406</t>
+  </si>
+  <si>
+    <t>32.815</t>
+  </si>
+  <si>
+    <t>29.22650</t>
+  </si>
+  <si>
+    <t>8.84408</t>
+  </si>
+  <si>
+    <t>8.84584</t>
+  </si>
+  <si>
+    <t>14.70392</t>
+  </si>
+  <si>
+    <t>14.70396</t>
+  </si>
+  <si>
+    <t>2.97361</t>
+  </si>
+  <si>
+    <t>33.35217</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -8797,7 +8893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8834,13 +8930,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9157,8 +9262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A8D13D-CD48-6440-9AB3-0F39AA71FBF9}">
   <dimension ref="A1:G882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A726" workbookViewId="0">
-      <selection activeCell="G736" sqref="G736"/>
+    <sheetView topLeftCell="A289" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B297" sqref="B297:F297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25466,7 +25571,7 @@
       </c>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A738" s="28" t="s">
+      <c r="A738" s="26" t="s">
         <v>2850</v>
       </c>
       <c r="B738" s="3">
@@ -25488,7 +25593,7 @@
       </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A739" s="28" t="s">
+      <c r="A739" s="26" t="s">
         <v>2851</v>
       </c>
       <c r="B739" s="3">
@@ -25510,7 +25615,7 @@
       </c>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A740" s="28" t="s">
+      <c r="A740" s="26" t="s">
         <v>2852</v>
       </c>
       <c r="B740" s="3">
@@ -25532,7 +25637,7 @@
       </c>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A741" s="28" t="s">
+      <c r="A741" s="26" t="s">
         <v>2853</v>
       </c>
       <c r="B741" s="3">
@@ -25554,7 +25659,7 @@
       </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A742" s="28" t="s">
+      <c r="A742" s="26" t="s">
         <v>2854</v>
       </c>
       <c r="B742" s="3">
@@ -25576,7 +25681,7 @@
       </c>
     </row>
     <row r="743" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A743" s="28" t="s">
+      <c r="A743" s="26" t="s">
         <v>2855</v>
       </c>
       <c r="B743" s="3">
@@ -25598,7 +25703,7 @@
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A744" s="28" t="s">
+      <c r="A744" s="26" t="s">
         <v>2856</v>
       </c>
       <c r="B744" s="3">
@@ -25620,7 +25725,7 @@
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A745" s="28" t="s">
+      <c r="A745" s="26" t="s">
         <v>2857</v>
       </c>
       <c r="B745" s="3">
@@ -25642,7 +25747,7 @@
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A746" s="28" t="s">
+      <c r="A746" s="26" t="s">
         <v>2858</v>
       </c>
       <c r="B746" s="3">
@@ -25664,7 +25769,7 @@
       </c>
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A747" s="28" t="s">
+      <c r="A747" s="26" t="s">
         <v>2859</v>
       </c>
       <c r="B747" s="3">
@@ -25686,7 +25791,7 @@
       </c>
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A748" s="28" t="s">
+      <c r="A748" s="26" t="s">
         <v>2860</v>
       </c>
       <c r="B748" s="3">
@@ -25708,7 +25813,7 @@
       </c>
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A749" s="28" t="s">
+      <c r="A749" s="26" t="s">
         <v>2861</v>
       </c>
       <c r="B749" s="3">
@@ -25730,7 +25835,7 @@
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A750" s="28" t="s">
+      <c r="A750" s="26" t="s">
         <v>2862</v>
       </c>
       <c r="B750" s="3">
@@ -25752,7 +25857,7 @@
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A751" s="28" t="s">
+      <c r="A751" s="26" t="s">
         <v>2863</v>
       </c>
       <c r="B751" s="3">
@@ -28662,6 +28767,737 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD796437-94FF-804A-B5A6-7FFEA47A7F30}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1" t="s">
+        <v>718</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B2">
+        <v>139741252</v>
+      </c>
+      <c r="C2">
+        <v>0.59845000000000004</v>
+      </c>
+      <c r="D2">
+        <v>-35.121220000000001</v>
+      </c>
+      <c r="E2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2">
+        <v>0.51</v>
+      </c>
+      <c r="G2">
+        <v>19.2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="B3">
+        <v>139823797</v>
+      </c>
+      <c r="C3">
+        <v>0.81825000000000003</v>
+      </c>
+      <c r="D3">
+        <v>-33.801200000000001</v>
+      </c>
+      <c r="E3">
+        <v>2.7</v>
+      </c>
+      <c r="F3">
+        <v>0.68</v>
+      </c>
+      <c r="G3">
+        <v>19.3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>142775105</v>
+      </c>
+      <c r="C4">
+        <v>1.6859200000000001</v>
+      </c>
+      <c r="D4">
+        <v>-44.497349999999997</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0.53</v>
+      </c>
+      <c r="G4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>142779522</v>
+      </c>
+      <c r="C5">
+        <v>1.87201</v>
+      </c>
+      <c r="D5">
+        <v>-44.57949</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.52</v>
+      </c>
+      <c r="G5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B6">
+        <v>182452355</v>
+      </c>
+      <c r="C6">
+        <v>2.6267800000000001</v>
+      </c>
+      <c r="D6">
+        <v>-43.254130000000004</v>
+      </c>
+      <c r="E6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.84</v>
+      </c>
+      <c r="G6">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>182003535</v>
+      </c>
+      <c r="C7">
+        <v>2.9713500000000002</v>
+      </c>
+      <c r="D7">
+        <v>-46.239420000000003</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0.6</v>
+      </c>
+      <c r="G7">
+        <v>18.5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B8">
+        <v>179698697</v>
+      </c>
+      <c r="C8">
+        <v>3.2901600000000002</v>
+      </c>
+      <c r="D8">
+        <v>0.66766999999999999</v>
+      </c>
+      <c r="E8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.75</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>140003287</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>29.66</v>
+      </c>
+      <c r="F9">
+        <v>-52</v>
+      </c>
+      <c r="G9">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>141268015</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>41.13</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>52.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>142078524</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>38.47</v>
+      </c>
+      <c r="F11">
+        <v>-51</v>
+      </c>
+      <c r="G11">
+        <v>55</v>
+      </c>
+      <c r="H11">
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>142345819</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>28.14</v>
+      </c>
+      <c r="F12">
+        <v>-38</v>
+      </c>
+      <c r="G12">
+        <v>44</v>
+      </c>
+      <c r="H12">
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>182976851</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>10.34</v>
+      </c>
+      <c r="F13">
+        <v>-55</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>50.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
+        <v>182217410</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>25.41</v>
+      </c>
+      <c r="F14">
+        <v>-54</v>
+      </c>
+      <c r="G14">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>33.770000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
+        <v>182434686</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>35.18</v>
+      </c>
+      <c r="F15">
+        <v>-39</v>
+      </c>
+      <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>717</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B18" s="12">
+        <v>139741252</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.59845000000000004</v>
+      </c>
+      <c r="D18" s="12">
+        <v>-35.121220000000001</v>
+      </c>
+      <c r="E18" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.51</v>
+      </c>
+      <c r="G18" s="12">
+        <v>19.2</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="B19" s="12">
+        <v>139823797</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.81825000000000003</v>
+      </c>
+      <c r="D19" s="12">
+        <v>-33.801200000000001</v>
+      </c>
+      <c r="E19" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0.68</v>
+      </c>
+      <c r="G19" s="12">
+        <v>19.3</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="12">
+        <v>142775105</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1.6859200000000001</v>
+      </c>
+      <c r="D20" s="12">
+        <v>-44.497349999999997</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="G20" s="12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="12">
+        <v>142779522</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1.87201</v>
+      </c>
+      <c r="D21" s="12">
+        <v>-44.57949</v>
+      </c>
+      <c r="E21" s="12">
+        <v>3</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="G21" s="12">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B22" s="12">
+        <v>182452355</v>
+      </c>
+      <c r="C22" s="12">
+        <v>2.6267800000000001</v>
+      </c>
+      <c r="D22" s="12">
+        <v>-43.254130000000004</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="G22" s="12">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="12">
+        <v>182003535</v>
+      </c>
+      <c r="C23" s="12">
+        <v>2.9713500000000002</v>
+      </c>
+      <c r="D23" s="12">
+        <v>-46.239420000000003</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="G23" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>1105</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B24" s="12">
+        <v>179698697</v>
+      </c>
+      <c r="C24" s="12">
+        <v>3.2901600000000002</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.66766999999999999</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="G24" s="12">
+        <v>20</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="14">
+        <v>140003287</v>
+      </c>
+      <c r="C25" s="12">
+        <f>((C9)+(D9/60)+(E9/3600))*15</f>
+        <v>0.62358333333333327</v>
+      </c>
+      <c r="D25" s="12">
+        <f>F9-(G9/60)-(H9/3600)</f>
+        <v>-52.488861111111113</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="14">
+        <v>141268015</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" ref="C26:C31" si="0">((C10)+(D10/60)+(E10/3600))*15</f>
+        <v>0.67137499999999994</v>
+      </c>
+      <c r="D26" s="12">
+        <f t="shared" ref="D26" si="1">F10+(G10/60)+(H10/3600)</f>
+        <v>2.8146805555555554</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="14">
+        <v>142078524</v>
+      </c>
+      <c r="C27" s="12">
+        <f t="shared" si="0"/>
+        <v>0.91029166666666672</v>
+      </c>
+      <c r="D27" s="12">
+        <f>F11-(G11/60)-(H11/3600)</f>
+        <v>-51.932611111111108</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="14">
+        <v>142345819</v>
+      </c>
+      <c r="C28" s="12">
+        <f t="shared" si="0"/>
+        <v>1.1172500000000001</v>
+      </c>
+      <c r="D28" s="12">
+        <f>F12-(G12/60)-(H12/3600)</f>
+        <v>-38.735819444444445</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="14">
+        <v>182976851</v>
+      </c>
+      <c r="C29" s="12">
+        <f t="shared" si="0"/>
+        <v>1.5430833333333334</v>
+      </c>
+      <c r="D29" s="12">
+        <f>F13-(G13/60)-(H13/3600)</f>
+        <v>-55.130580555555554</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="14">
+        <v>182217410</v>
+      </c>
+      <c r="C30" s="12">
+        <f t="shared" si="0"/>
+        <v>1.6058750000000002</v>
+      </c>
+      <c r="D30" s="12">
+        <f>F14-(G14/60)-(H14/3600)</f>
+        <v>-54.409380555555558</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16">
+        <v>182434686</v>
+      </c>
+      <c r="C31" s="12">
+        <f t="shared" si="0"/>
+        <v>2.1465833333333331</v>
+      </c>
+      <c r="D31" s="17">
+        <f>F15-(G15/60)-(H15/3600)</f>
+        <v>-39.377361111111114</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BEB169-96F4-734C-8A73-9828CC2B5F75}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28673,7 +29509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F87BBA-BC16-DD40-96FA-DA2C592E0EA9}">
   <dimension ref="A1:K229"/>
   <sheetViews>
@@ -36786,6 +37622,568 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7EA1A4-C11E-4841-99DA-F5C1C183EC45}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="18.33203125" style="12"/>
+    <col min="3" max="3" width="18.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="18.33203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="29">
+        <v>268</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2866</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>2888</v>
+      </c>
+      <c r="D2" s="31">
+        <v>-4.4070999999999998</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>43</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>2867</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>2889</v>
+      </c>
+      <c r="D3" s="31">
+        <v>-51.503093</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="29">
+        <v>162</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>2868</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>692</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0.1958</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="F4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="29">
+        <v>296</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>2869</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D5" s="31">
+        <v>-1.4632000000000001</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="29">
+        <v>41</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>2867</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>2890</v>
+      </c>
+      <c r="D6" s="31">
+        <v>-51.506618000000003</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>751</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>2870</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>2891</v>
+      </c>
+      <c r="D7" s="31">
+        <v>-7.3657500000000002</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>2848</v>
+      </c>
+      <c r="F7" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="29">
+        <v>781</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>2870</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>2892</v>
+      </c>
+      <c r="D8" s="31">
+        <v>-7.3657500000000002</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>2848</v>
+      </c>
+      <c r="F8" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>79</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>2871</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9" s="31">
+        <v>2.4285999999999999</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="F9" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>211</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>2872</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>2886</v>
+      </c>
+      <c r="D10" s="31">
+        <v>-36.177700000000002</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F10" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>17</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>2873</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>2893</v>
+      </c>
+      <c r="D11" s="31">
+        <v>-46.239201000000001</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="29">
+        <v>563</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>2874</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>2894</v>
+      </c>
+      <c r="D12" s="31">
+        <v>-7.73189444444444</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F12" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>274</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>2875</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>2887</v>
+      </c>
+      <c r="D13" s="31">
+        <v>-3.7299000000000002</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>473</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>2871</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="D14" s="31">
+        <v>2.4285999999999999</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>461</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>2876</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D15" s="31">
+        <v>-0.32640000000000002</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>690</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>2877</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0</v>
+      </c>
+      <c r="D16" s="31">
+        <v>2.4152777777777801</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F16" s="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="29">
+        <v>598</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>2878</v>
+      </c>
+      <c r="C17" s="31">
+        <v>37.666499999999999</v>
+      </c>
+      <c r="D17" s="31">
+        <v>-3.8411277777777801</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F17" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>28</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>2879</v>
+      </c>
+      <c r="C18" s="31">
+        <v>5.9326999999999996</v>
+      </c>
+      <c r="D18" s="31">
+        <v>-49.390300000000003</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F18" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="29">
+        <v>25</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>2880</v>
+      </c>
+      <c r="C19" s="31">
+        <v>5.4518310000000003</v>
+      </c>
+      <c r="D19" s="31">
+        <v>-50.474888</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="29">
+        <v>879</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>2868</v>
+      </c>
+      <c r="C20" s="31">
+        <v>340.50491666666699</v>
+      </c>
+      <c r="D20" s="31">
+        <v>2.4696138888888899</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>574</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>2881</v>
+      </c>
+      <c r="C21" s="31">
+        <v>34.414833333333299</v>
+      </c>
+      <c r="D21" s="31">
+        <v>-10.555536111111101</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F21" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
+        <v>27</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>2879</v>
+      </c>
+      <c r="C22" s="31">
+        <v>5.9334790000000002</v>
+      </c>
+      <c r="D22" s="31">
+        <v>-49.391714</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F22" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>667</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>2882</v>
+      </c>
+      <c r="C23" s="31">
+        <v>333.57841666666701</v>
+      </c>
+      <c r="D23" s="31">
+        <v>1.1760694444444399</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F23" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>18</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>2873</v>
+      </c>
+      <c r="C24" s="31">
+        <v>2.9729830000000002</v>
+      </c>
+      <c r="D24" s="31">
+        <v>-46.238663000000003</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F24" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="29">
+        <v>5</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>2883</v>
+      </c>
+      <c r="C25" s="31">
+        <v>1.512545</v>
+      </c>
+      <c r="D25" s="31">
+        <v>-42.139282999999999</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>31</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>2884</v>
+      </c>
+      <c r="C26" s="31">
+        <v>6.4905910000000002</v>
+      </c>
+      <c r="D26" s="31">
+        <v>-41.555939000000002</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>347</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>2869</v>
+      </c>
+      <c r="C27" s="31">
+        <v>39.926000000000002</v>
+      </c>
+      <c r="D27" s="31">
+        <v>-1.4632000000000001</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9983360C-B04E-264E-A2FD-A3AF9B5DD60B}">
   <dimension ref="A1:T81"/>
   <sheetViews>
@@ -41103,7 +42501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93146DE-552A-8643-8297-5506E5980AEB}">
   <dimension ref="A1:R258"/>
   <sheetViews>
@@ -41117,16 +42515,16 @@
       <c r="A1" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="34" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
         <v>1108</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" t="s">
         <v>2357</v>
       </c>
@@ -51987,12 +53385,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D4FBA8-32E1-0947-8594-D9135F20884A}">
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView topLeftCell="A78" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52022,16 +53420,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -54849,7 +56247,7 @@
       <c r="A91" s="21" t="s">
         <v>2220</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -55465,7 +56863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D17124-76D0-7141-B43B-9234C48820EB}">
   <dimension ref="A1:E47"/>
   <sheetViews>
@@ -56288,7 +57686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4DC53C-CD95-F84B-8217-D56E75606B8F}">
   <dimension ref="A1:V52"/>
   <sheetViews>
@@ -59477,7 +60875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31C520D-257B-3141-B803-1F468B25B845}">
   <dimension ref="A1:O186"/>
   <sheetViews>
@@ -64642,7 +66040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691D74B0-5132-BD40-A45B-EA0D74212FE0}">
   <dimension ref="A1:H85"/>
   <sheetViews>
@@ -64682,10 +66080,10 @@
       <c r="F1" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="35" t="s">
         <v>719</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -66877,735 +68275,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD796437-94FF-804A-B5A6-7FFEA47A7F30}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="B1" t="s">
-        <v>717</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G1" t="s">
-        <v>718</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B2">
-        <v>139741252</v>
-      </c>
-      <c r="C2">
-        <v>0.59845000000000004</v>
-      </c>
-      <c r="D2">
-        <v>-35.121220000000001</v>
-      </c>
-      <c r="E2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F2">
-        <v>0.51</v>
-      </c>
-      <c r="G2">
-        <v>19.2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="B3">
-        <v>139823797</v>
-      </c>
-      <c r="C3">
-        <v>0.81825000000000003</v>
-      </c>
-      <c r="D3">
-        <v>-33.801200000000001</v>
-      </c>
-      <c r="E3">
-        <v>2.7</v>
-      </c>
-      <c r="F3">
-        <v>0.68</v>
-      </c>
-      <c r="G3">
-        <v>19.3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>142775105</v>
-      </c>
-      <c r="C4">
-        <v>1.6859200000000001</v>
-      </c>
-      <c r="D4">
-        <v>-44.497349999999997</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>0.53</v>
-      </c>
-      <c r="G4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>142779522</v>
-      </c>
-      <c r="C5">
-        <v>1.87201</v>
-      </c>
-      <c r="D5">
-        <v>-44.57949</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>0.52</v>
-      </c>
-      <c r="G5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B6">
-        <v>182452355</v>
-      </c>
-      <c r="C6">
-        <v>2.6267800000000001</v>
-      </c>
-      <c r="D6">
-        <v>-43.254130000000004</v>
-      </c>
-      <c r="E6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F6">
-        <v>0.84</v>
-      </c>
-      <c r="G6">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7">
-        <v>182003535</v>
-      </c>
-      <c r="C7">
-        <v>2.9713500000000002</v>
-      </c>
-      <c r="D7">
-        <v>-46.239420000000003</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>0.6</v>
-      </c>
-      <c r="G7">
-        <v>18.5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1105</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B8">
-        <v>179698697</v>
-      </c>
-      <c r="C8">
-        <v>3.2901600000000002</v>
-      </c>
-      <c r="D8">
-        <v>0.66766999999999999</v>
-      </c>
-      <c r="E8">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F8">
-        <v>0.75</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
-        <v>140003287</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>29.66</v>
-      </c>
-      <c r="F9">
-        <v>-52</v>
-      </c>
-      <c r="G9">
-        <v>29</v>
-      </c>
-      <c r="H9">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <v>141268015</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>41.13</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>48</v>
-      </c>
-      <c r="H10">
-        <v>52.85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
-        <v>142078524</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>38.47</v>
-      </c>
-      <c r="F11">
-        <v>-51</v>
-      </c>
-      <c r="G11">
-        <v>55</v>
-      </c>
-      <c r="H11">
-        <v>57.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
-        <v>142345819</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>28.14</v>
-      </c>
-      <c r="F12">
-        <v>-38</v>
-      </c>
-      <c r="G12">
-        <v>44</v>
-      </c>
-      <c r="H12">
-        <v>8.9499999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
-        <v>182976851</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>10.34</v>
-      </c>
-      <c r="F13">
-        <v>-55</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>50.09</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
-        <v>182217410</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>25.41</v>
-      </c>
-      <c r="F14">
-        <v>-54</v>
-      </c>
-      <c r="G14">
-        <v>24</v>
-      </c>
-      <c r="H14">
-        <v>33.770000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="2">
-        <v>182434686</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>35.18</v>
-      </c>
-      <c r="F15">
-        <v>-39</v>
-      </c>
-      <c r="G15">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>717</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>718</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B18" s="12">
-        <v>139741252</v>
-      </c>
-      <c r="C18" s="12">
-        <v>0.59845000000000004</v>
-      </c>
-      <c r="D18" s="12">
-        <v>-35.121220000000001</v>
-      </c>
-      <c r="E18" s="12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0.51</v>
-      </c>
-      <c r="G18" s="12">
-        <v>19.2</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>720</v>
-      </c>
-      <c r="B19" s="12">
-        <v>139823797</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0.81825000000000003</v>
-      </c>
-      <c r="D19" s="12">
-        <v>-33.801200000000001</v>
-      </c>
-      <c r="E19" s="12">
-        <v>2.7</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.68</v>
-      </c>
-      <c r="G19" s="12">
-        <v>19.3</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="12">
-        <v>142775105</v>
-      </c>
-      <c r="C20" s="12">
-        <v>1.6859200000000001</v>
-      </c>
-      <c r="D20" s="12">
-        <v>-44.497349999999997</v>
-      </c>
-      <c r="E20" s="12">
-        <v>2</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0.53</v>
-      </c>
-      <c r="G20" s="12">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="12">
-        <v>142779522</v>
-      </c>
-      <c r="C21" s="12">
-        <v>1.87201</v>
-      </c>
-      <c r="D21" s="12">
-        <v>-44.57949</v>
-      </c>
-      <c r="E21" s="12">
-        <v>3</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0.52</v>
-      </c>
-      <c r="G21" s="12">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B22" s="12">
-        <v>182452355</v>
-      </c>
-      <c r="C22" s="12">
-        <v>2.6267800000000001</v>
-      </c>
-      <c r="D22" s="12">
-        <v>-43.254130000000004</v>
-      </c>
-      <c r="E22" s="12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="G22" s="12">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>1104</v>
-      </c>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="12">
-        <v>182003535</v>
-      </c>
-      <c r="C23" s="12">
-        <v>2.9713500000000002</v>
-      </c>
-      <c r="D23" s="12">
-        <v>-46.239420000000003</v>
-      </c>
-      <c r="E23" s="12">
-        <v>3</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="G23" s="12">
-        <v>18.5</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>1105</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B24" s="12">
-        <v>179698697</v>
-      </c>
-      <c r="C24" s="12">
-        <v>3.2901600000000002</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0.66766999999999999</v>
-      </c>
-      <c r="E24" s="12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0.75</v>
-      </c>
-      <c r="G24" s="12">
-        <v>20</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="14">
-        <v>140003287</v>
-      </c>
-      <c r="C25" s="12">
-        <f>((C9)+(D9/60)+(E9/3600))*15</f>
-        <v>0.62358333333333327</v>
-      </c>
-      <c r="D25" s="12">
-        <f>F9-(G9/60)-(H9/3600)</f>
-        <v>-52.488861111111113</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14">
-        <v>141268015</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" ref="C26:C31" si="0">((C10)+(D10/60)+(E10/3600))*15</f>
-        <v>0.67137499999999994</v>
-      </c>
-      <c r="D26" s="12">
-        <f t="shared" ref="D26" si="1">F10+(G10/60)+(H10/3600)</f>
-        <v>2.8146805555555554</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="14">
-        <v>142078524</v>
-      </c>
-      <c r="C27" s="12">
-        <f t="shared" si="0"/>
-        <v>0.91029166666666672</v>
-      </c>
-      <c r="D27" s="12">
-        <f>F11-(G11/60)-(H11/3600)</f>
-        <v>-51.932611111111108</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="14">
-        <v>142345819</v>
-      </c>
-      <c r="C28" s="12">
-        <f t="shared" si="0"/>
-        <v>1.1172500000000001</v>
-      </c>
-      <c r="D28" s="12">
-        <f>F12-(G12/60)-(H12/3600)</f>
-        <v>-38.735819444444445</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14">
-        <v>182976851</v>
-      </c>
-      <c r="C29" s="12">
-        <f t="shared" si="0"/>
-        <v>1.5430833333333334</v>
-      </c>
-      <c r="D29" s="12">
-        <f>F13-(G13/60)-(H13/3600)</f>
-        <v>-55.130580555555554</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14">
-        <v>182217410</v>
-      </c>
-      <c r="C30" s="12">
-        <f t="shared" si="0"/>
-        <v>1.6058750000000002</v>
-      </c>
-      <c r="D30" s="12">
-        <f>F14-(G14/60)-(H14/3600)</f>
-        <v>-54.409380555555558</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="13"/>
-    </row>
-    <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16">
-        <v>182434686</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="0"/>
-        <v>2.1465833333333331</v>
-      </c>
-      <c r="D31" s="17">
-        <f>F15-(G15/60)-(H15/3600)</f>
-        <v>-39.377361111111114</v>
-      </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding predicted lenses to the spreadsheet
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68014148-7B56-D14D-8D37-4B9B3C69A850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49089F55-4783-6947-81CA-C671BE8C5C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8398" uniqueCount="2921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8473" uniqueCount="2953">
   <si>
     <t>PAPER_TILE</t>
   </si>
@@ -8808,6 +8808,102 @@
   </si>
   <si>
     <t xml:space="preserve"> 583_DES0222-1041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">284_DES0223-0333 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 690_DES0000+0209 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 449_DES2214+0126 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 283_DES0223-0333 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 264_DES0031+0043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43_DES0035-5123 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">315_DES0031+0043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 440_DES2208+0209 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 288_DES0231-0207 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 579_DES0219-1041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 266_DES0108+0126 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 243_DES0148-0250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 270_DES0201-0416 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35_DES0030-4414 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19_DES0011-4623 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 284_DES0223-0333 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11_DES0008-5457 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_DES0008-5457 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 315_DES0031+0043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 294_DES0148-0250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 589_DES0223-0416 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 491_DES0223-0416 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 598_DES0232-0333 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 263_DES0014-0041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42_DES0035-5123 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 458_DES2231+0043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 574_DES0216-1041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18_DES0011-4623 </t>
+  </si>
+  <si>
+    <t>Found in 3</t>
+  </si>
+  <si>
+    <t>Found in 2</t>
+  </si>
+  <si>
+    <t>Found in 1</t>
+  </si>
+  <si>
+    <t>Found in all 4</t>
   </si>
 </sst>
 </file>
@@ -40501,24 +40597,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976FD3A7-3202-C743-846D-2E8ADD6ECC71}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C1" s="26" t="s">
         <v>717</v>
       </c>
@@ -40535,8 +40639,20 @@
         <v>2864</v>
       </c>
       <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>2951</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2950</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2949</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2895</v>
       </c>
@@ -40558,8 +40674,23 @@
       <c r="H2" s="30">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2896</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2907</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2895</v>
+      </c>
+      <c r="T2" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2896</v>
       </c>
@@ -40569,8 +40700,20 @@
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
       <c r="H3" s="26"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>2922</v>
+      </c>
+      <c r="R3" t="s">
+        <v>2911</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2904</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2897</v>
       </c>
@@ -40580,8 +40723,20 @@
       <c r="F4" s="27"/>
       <c r="G4" s="28"/>
       <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>2941</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2918</v>
+      </c>
+      <c r="S4" t="s">
+        <v>2909</v>
+      </c>
+      <c r="T4" t="s">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2898</v>
       </c>
@@ -40603,8 +40758,23 @@
       <c r="H5" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>2928</v>
+      </c>
+      <c r="N5" t="s">
+        <v>2925</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2920</v>
+      </c>
+      <c r="S5" t="s">
+        <v>2919</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2899</v>
       </c>
@@ -40626,8 +40796,20 @@
       <c r="H6" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>2922</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2929</v>
+      </c>
+      <c r="N6" t="s">
+        <v>2942</v>
+      </c>
+      <c r="T6" t="s">
+        <v>2901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2900</v>
       </c>
@@ -40637,8 +40819,14 @@
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>2924</v>
+      </c>
+      <c r="T7" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2901</v>
       </c>
@@ -40648,8 +40836,17 @@
       <c r="F8" s="27"/>
       <c r="G8" s="28"/>
       <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>2923</v>
+      </c>
+      <c r="N8" t="s">
+        <v>2943</v>
+      </c>
+      <c r="T8" t="s">
+        <v>2903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2902</v>
       </c>
@@ -40671,8 +40868,11 @@
       <c r="H9" s="30">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>2905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2903</v>
       </c>
@@ -40694,8 +40894,14 @@
       <c r="H10" s="30">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>2925</v>
+      </c>
+      <c r="T10" t="s">
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2904</v>
       </c>
@@ -40705,8 +40911,11 @@
       <c r="F11" s="27"/>
       <c r="G11" s="28"/>
       <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>2908</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2905</v>
       </c>
@@ -40728,8 +40937,17 @@
       <c r="H12" s="30">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>2930</v>
+      </c>
+      <c r="N12" t="s">
+        <v>2928</v>
+      </c>
+      <c r="T12" t="s">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2906</v>
       </c>
@@ -40739,8 +40957,11 @@
       <c r="F13" s="27"/>
       <c r="G13" s="28"/>
       <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="T13" t="s">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2907</v>
       </c>
@@ -40750,8 +40971,14 @@
       <c r="F14" s="27"/>
       <c r="G14" s="28"/>
       <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>2924</v>
+      </c>
+      <c r="T14" t="s">
+        <v>2913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2908</v>
       </c>
@@ -40773,8 +41000,11 @@
       <c r="H15" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2909</v>
       </c>
@@ -40796,8 +41026,11 @@
       <c r="H16" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="T16" t="s">
+        <v>2915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2910</v>
       </c>
@@ -40819,8 +41052,14 @@
       <c r="H17" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>2931</v>
+      </c>
+      <c r="T17" t="s">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2911</v>
       </c>
@@ -40830,8 +41069,11 @@
       <c r="F18" s="27"/>
       <c r="G18" s="28"/>
       <c r="H18" s="26"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>2924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2912</v>
       </c>
@@ -40842,7 +41084,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2913</v>
       </c>
@@ -40864,8 +41106,11 @@
       <c r="H20" s="30">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2914</v>
       </c>
@@ -40887,8 +41132,14 @@
       <c r="H21" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>2925</v>
+      </c>
+      <c r="L21" t="s">
+        <v>2932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2915</v>
       </c>
@@ -40910,8 +41161,14 @@
       <c r="H22" s="30">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>2933</v>
+      </c>
+      <c r="N22" t="s">
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2916</v>
       </c>
@@ -40933,8 +41190,14 @@
       <c r="H23" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>2934</v>
+      </c>
+      <c r="N23" t="s">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2917</v>
       </c>
@@ -40956,8 +41219,11 @@
       <c r="H24" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2918</v>
       </c>
@@ -40979,8 +41245,17 @@
       <c r="H25" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>2926</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2935</v>
+      </c>
+      <c r="N25" t="s">
+        <v>2946</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2919</v>
       </c>
@@ -40990,8 +41265,11 @@
       <c r="F26" s="27"/>
       <c r="G26" s="28"/>
       <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>2922</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2920</v>
       </c>
@@ -41001,32 +41279,44 @@
       <c r="F27" s="27"/>
       <c r="G27" s="28"/>
       <c r="H27" s="26"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>2923</v>
+      </c>
+      <c r="N27" t="s">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="5"/>
       <c r="H29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>2927</v>
+      </c>
+      <c r="L29" t="s">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="31"/>
@@ -41034,23 +41324,29 @@
       <c r="G31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="30"/>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
       <c r="G33" s="5"/>
       <c r="H33" s="30"/>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>2919</v>
+      </c>
+      <c r="N33" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="31"/>
@@ -41058,87 +41354,117 @@
       <c r="G34" s="5"/>
       <c r="H34" s="30"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="31"/>
       <c r="F35" s="31"/>
       <c r="G35" s="5"/>
       <c r="H35" s="30"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>2948</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
       <c r="E36" s="31"/>
       <c r="F36" s="31"/>
-      <c r="G36" s="7"/>
+      <c r="G36" s="5"/>
       <c r="H36" s="30"/>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="12"/>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G37" s="7"/>
+      <c r="H37" s="30"/>
+      <c r="N37" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="30"/>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="31"/>
       <c r="F39" s="31"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="30"/>
+      <c r="L39" t="s">
+        <v>2938</v>
+      </c>
+      <c r="N39" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="31"/>
       <c r="F40" s="31"/>
       <c r="G40" s="5"/>
       <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
       <c r="G41" s="5"/>
       <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>2908</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="31"/>
       <c r="F42" s="31"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="30"/>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H42" s="12"/>
+      <c r="L42" t="s">
+        <v>2934</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="5"/>
       <c r="H43" s="30"/>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L43" t="s">
+        <v>2932</v>
+      </c>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="31"/>
       <c r="F44" s="31"/>
-      <c r="G44" s="6"/>
+      <c r="G44" s="5"/>
       <c r="H44" s="30"/>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="31"/>
@@ -41146,29 +41472,32 @@
       <c r="G45" s="6"/>
       <c r="H45" s="30"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="30"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
       <c r="G47" s="5"/>
       <c r="H47" s="30"/>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
       <c r="G48" s="5"/>
-      <c r="H48" s="12"/>
+      <c r="H48" s="30"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C49" s="29"/>
@@ -41176,7 +41505,7 @@
       <c r="E49" s="31"/>
       <c r="F49" s="31"/>
       <c r="G49" s="5"/>
-      <c r="H49" s="30"/>
+      <c r="H49" s="12"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C50" s="29"/>
@@ -41184,7 +41513,7 @@
       <c r="E50" s="31"/>
       <c r="F50" s="31"/>
       <c r="G50" s="5"/>
-      <c r="H50" s="12"/>
+      <c r="H50" s="30"/>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C51" s="29"/>
@@ -41199,16 +41528,24 @@
       <c r="D52" s="29"/>
       <c r="E52" s="31"/>
       <c r="F52" s="31"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="30"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="12"/>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="31"/>
       <c r="F53" s="31"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="12"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="30"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commiting the Unseen Known Lenses
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A92FB53-16DE-9041-8D34-F7F02EDE7697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC7B53C-1D51-0744-89E3-BD7804808988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
@@ -29,7 +29,6 @@
     <sheet name="Jae20" sheetId="8" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -9018,7 +9017,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -9247,15 +9246,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -34282,10 +34281,10 @@
       <c r="F1" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="43" t="s">
         <v>719</v>
       </c>
-      <c r="H1" s="40"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -45338,8 +45337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976FD3A7-3202-C743-846D-2E8ADD6ECC71}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:L49"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45414,13 +45413,13 @@
       <c r="F2" t="s">
         <v>2715</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="41">
         <v>14.70392</v>
       </c>
       <c r="H2" t="s">
         <v>2715</v>
       </c>
-      <c r="I2" s="43">
+      <c r="I2" s="41">
         <v>-7.3657500000000002</v>
       </c>
       <c r="J2" t="s">
@@ -45429,7 +45428,7 @@
       <c r="K2" s="30">
         <v>4</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M2" s="5" t="s">
@@ -45467,13 +45466,13 @@
       <c r="F3" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="41">
         <v>33.288600000000002</v>
       </c>
       <c r="H3" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="41">
         <v>-24.229199999999999</v>
       </c>
       <c r="J3" s="29" t="s">
@@ -45482,7 +45481,7 @@
       <c r="K3">
         <v>5</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M3" s="7" t="s">
@@ -45520,13 +45519,13 @@
       <c r="F4" t="s">
         <v>2715</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="41">
         <v>2.9728940000000001</v>
       </c>
       <c r="H4" t="s">
         <v>2715</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="41">
         <v>-46.241202000000001</v>
       </c>
       <c r="J4" t="s">
@@ -45535,7 +45534,7 @@
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -45573,13 +45572,13 @@
       <c r="F5" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="41">
         <v>333.57841666666701</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="41">
         <v>1.1760694444444399</v>
       </c>
       <c r="J5" s="29" t="s">
@@ -45588,7 +45587,7 @@
       <c r="K5" s="30">
         <v>6</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="L5" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M5" s="5" t="s">
@@ -45626,13 +45625,13 @@
       <c r="F6" t="s">
         <v>2715</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="41">
         <v>346.74279999999999</v>
       </c>
       <c r="H6" t="s">
         <v>2715</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="41">
         <v>2.4285999999999999</v>
       </c>
       <c r="J6" t="s">
@@ -45641,7 +45640,7 @@
       <c r="K6" s="12">
         <v>1</v>
       </c>
-      <c r="L6" s="41" t="s">
+      <c r="L6" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M6" s="5" t="s">
@@ -45679,13 +45678,13 @@
       <c r="F7" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="41">
         <v>349.9726</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="41">
         <v>0.63690000000000002</v>
       </c>
       <c r="J7" s="29" t="s">
@@ -45694,7 +45693,7 @@
       <c r="K7" s="30">
         <v>1</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M7" s="5" t="s">
@@ -45732,13 +45731,13 @@
       <c r="F8" t="s">
         <v>2715</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="41">
         <v>5.9326999999999996</v>
       </c>
       <c r="H8" t="s">
         <v>2715</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="41">
         <v>-49.390300000000003</v>
       </c>
       <c r="J8" t="s">
@@ -45747,7 +45746,7 @@
       <c r="K8" s="30">
         <v>2</v>
       </c>
-      <c r="L8" s="41" t="s">
+      <c r="L8" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -45785,13 +45784,13 @@
       <c r="F9" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="41">
         <v>8.8458400000000008</v>
       </c>
       <c r="H9" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="41">
         <v>-51.506618000000003</v>
       </c>
       <c r="J9" s="29" t="s">
@@ -45800,7 +45799,7 @@
       <c r="K9" s="30">
         <v>2</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M9" s="5" t="s">
@@ -45838,13 +45837,13 @@
       <c r="F10" t="s">
         <v>2715</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="41">
         <v>48.405999999999999</v>
       </c>
       <c r="H10" t="s">
         <v>2715</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="41">
         <v>-36.177700000000002</v>
       </c>
       <c r="J10" t="s">
@@ -45853,7 +45852,7 @@
       <c r="K10" s="30">
         <v>5</v>
       </c>
-      <c r="L10" s="41" t="s">
+      <c r="L10" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M10" s="7" t="s">
@@ -45889,13 +45888,13 @@
       <c r="F11" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="41">
         <v>33.352166666666697</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="41">
         <v>-7.7318944444444444</v>
       </c>
       <c r="J11" s="29" t="s">
@@ -45904,7 +45903,7 @@
       <c r="K11" s="35">
         <v>6</v>
       </c>
-      <c r="L11" s="42" t="s">
+      <c r="L11" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M11" s="5" t="s">
@@ -45938,13 +45937,13 @@
       <c r="F12" t="s">
         <v>2715</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="41">
         <v>346.74279999999999</v>
       </c>
       <c r="H12" t="s">
         <v>2715</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I12" s="41">
         <v>2.4285999999999999</v>
       </c>
       <c r="J12" t="s">
@@ -45953,7 +45952,7 @@
       <c r="K12" s="30">
         <v>3</v>
       </c>
-      <c r="L12" s="41" t="s">
+      <c r="L12" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M12" s="5" t="s">
@@ -45987,13 +45986,13 @@
       <c r="F13" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="41">
         <v>6.4905910000000002</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I13" s="43">
+      <c r="I13" s="41">
         <v>-41.555939000000002</v>
       </c>
       <c r="J13" s="29" t="s">
@@ -46002,7 +46001,7 @@
       <c r="K13">
         <v>2</v>
       </c>
-      <c r="L13" s="42" t="s">
+      <c r="L13" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M13" s="6" t="s">
@@ -46036,13 +46035,13 @@
       <c r="F14" t="s">
         <v>2715</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="41">
         <v>5.3912000000000004</v>
       </c>
       <c r="H14" t="s">
         <v>2715</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="41">
         <v>-40.667900000000003</v>
       </c>
       <c r="J14" t="s">
@@ -46051,7 +46050,7 @@
       <c r="K14">
         <v>2</v>
       </c>
-      <c r="L14" s="41" t="s">
+      <c r="L14" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M14" s="6" t="s">
@@ -46085,13 +46084,13 @@
       <c r="F15" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="41">
         <v>2.9729830000000002</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="41">
         <v>-46.238663000000003</v>
       </c>
       <c r="J15" s="29" t="s">
@@ -46100,7 +46099,7 @@
       <c r="K15" s="12">
         <v>2</v>
       </c>
-      <c r="L15" s="42" t="s">
+      <c r="L15" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M15" s="5" t="s">
@@ -46134,13 +46133,13 @@
       <c r="F16" t="s">
         <v>2715</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="41">
         <v>32.814999999999998</v>
       </c>
       <c r="H16" t="s">
         <v>2715</v>
       </c>
-      <c r="I16" s="43">
+      <c r="I16" s="41">
         <v>-3.7299000000000002</v>
       </c>
       <c r="J16" t="s">
@@ -46149,7 +46148,7 @@
       <c r="K16" s="12">
         <v>1</v>
       </c>
-      <c r="L16" s="41" t="s">
+      <c r="L16" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M16" s="5" t="s">
@@ -46183,13 +46182,13 @@
       <c r="F17" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="41">
         <v>338.3331</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I17" s="43">
+      <c r="I17" s="41">
         <v>-0.32640000000000002</v>
       </c>
       <c r="J17" s="29" t="s">
@@ -46198,7 +46197,7 @@
       <c r="K17" s="12">
         <v>1</v>
       </c>
-      <c r="L17" s="42" t="s">
+      <c r="L17" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M17" s="5" t="s">
@@ -46230,13 +46229,13 @@
       <c r="F18" t="s">
         <v>2715</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="41">
         <v>33.533625000000001</v>
       </c>
       <c r="H18" t="s">
         <v>2715</v>
       </c>
-      <c r="I18" s="43">
+      <c r="I18" s="41">
         <v>-5.5923305555555549</v>
       </c>
       <c r="J18" t="s">
@@ -46245,7 +46244,7 @@
       <c r="K18">
         <v>6</v>
       </c>
-      <c r="L18" s="41" t="s">
+      <c r="L18" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M18" s="5" t="s">
@@ -46275,13 +46274,13 @@
       <c r="F19" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="41">
         <v>340.99900000000002</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I19" s="43">
+      <c r="I19" s="41">
         <v>-8.0299999999999996E-2</v>
       </c>
       <c r="J19" s="29" t="s">
@@ -46290,7 +46289,7 @@
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="L19" s="42" t="s">
+      <c r="L19" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M19" s="5" t="s">
@@ -46320,13 +46319,13 @@
       <c r="F20" t="s">
         <v>2715</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="41">
         <v>6.4905910000000002</v>
       </c>
       <c r="H20" t="s">
         <v>2715</v>
       </c>
-      <c r="I20" s="43">
+      <c r="I20" s="41">
         <v>-41.555939000000002</v>
       </c>
       <c r="J20" t="s">
@@ -46335,7 +46334,7 @@
       <c r="K20" s="30">
         <v>2</v>
       </c>
-      <c r="L20" s="41" t="s">
+      <c r="L20" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M20" s="6" t="s">
@@ -46365,13 +46364,13 @@
       <c r="F21" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G21" s="41">
         <v>5.9334790000000002</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I21" s="43">
+      <c r="I21" s="41">
         <v>-49.391714</v>
       </c>
       <c r="J21" s="29" t="s">
@@ -46380,7 +46379,7 @@
       <c r="K21" s="12">
         <v>2</v>
       </c>
-      <c r="L21" s="42" t="s">
+      <c r="L21" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M21" s="5" t="s">
@@ -46425,13 +46424,13 @@
       <c r="F22" t="s">
         <v>2715</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="41">
         <v>340.50491666666699</v>
       </c>
       <c r="H22" t="s">
         <v>2715</v>
       </c>
-      <c r="I22" s="43">
+      <c r="I22" s="41">
         <v>2.4696138888888899</v>
       </c>
       <c r="J22" t="s">
@@ -46440,7 +46439,7 @@
       <c r="K22" s="30">
         <v>8</v>
       </c>
-      <c r="L22" s="41" t="s">
+      <c r="L22" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M22" s="5" t="s">
@@ -46485,13 +46484,13 @@
       <c r="F23" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="41">
         <v>2.9736099999999999</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I23" s="43">
+      <c r="I23" s="41">
         <v>-46.239201000000001</v>
       </c>
       <c r="J23" s="29" t="s">
@@ -46500,7 +46499,7 @@
       <c r="K23" s="12">
         <v>2</v>
       </c>
-      <c r="L23" s="42" t="s">
+      <c r="L23" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M23" s="5" t="s">
@@ -46530,13 +46529,13 @@
       <c r="F24" t="s">
         <v>2715</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="41">
         <v>340.5899</v>
       </c>
       <c r="H24" t="s">
         <v>2715</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="41">
         <v>0.1958</v>
       </c>
       <c r="J24" t="s">
@@ -46545,7 +46544,7 @@
       <c r="K24" s="12">
         <v>3</v>
       </c>
-      <c r="L24" s="41" t="s">
+      <c r="L24" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M24" s="5" t="s">
@@ -46575,13 +46574,13 @@
       <c r="F25" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="41">
         <v>1.512545</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I25" s="43">
+      <c r="I25" s="41">
         <v>-42.139282999999999</v>
       </c>
       <c r="J25" s="29" t="s">
@@ -46590,7 +46589,7 @@
       <c r="K25" s="12">
         <v>2</v>
       </c>
-      <c r="L25" s="42" t="s">
+      <c r="L25" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M25" s="5" t="s">
@@ -46620,13 +46619,13 @@
       <c r="F26" t="s">
         <v>2715</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="41">
         <v>14.703958333333334</v>
       </c>
       <c r="H26" t="s">
         <v>2715</v>
       </c>
-      <c r="I26" s="43">
+      <c r="I26" s="41">
         <v>-7.3657499999999994</v>
       </c>
       <c r="J26" t="s">
@@ -46635,7 +46634,7 @@
       <c r="K26">
         <v>4</v>
       </c>
-      <c r="L26" s="41" t="s">
+      <c r="L26" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M26" s="5" t="s">
@@ -46665,13 +46664,13 @@
       <c r="F27" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="41">
         <v>35.826374999999999</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="41">
         <v>-10.980127777777778</v>
       </c>
       <c r="J27" s="29" t="s">
@@ -46680,7 +46679,7 @@
       <c r="K27">
         <v>6</v>
       </c>
-      <c r="L27" s="42" t="s">
+      <c r="L27" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M27" s="5" t="s">
@@ -46710,13 +46709,13 @@
       <c r="F28" t="s">
         <v>2715</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="41">
         <v>36.043700000000001</v>
       </c>
       <c r="H28" t="s">
         <v>2715</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="41">
         <v>-3.6015000000000001</v>
       </c>
       <c r="J28" t="s">
@@ -46725,7 +46724,7 @@
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="L28" s="41" t="s">
+      <c r="L28" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M28" s="5" t="s">
@@ -46755,13 +46754,13 @@
       <c r="F29" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G29" s="43">
+      <c r="G29" s="41">
         <v>0</v>
       </c>
       <c r="H29" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I29" s="43">
+      <c r="I29" s="41">
         <v>2.4152777777777779</v>
       </c>
       <c r="J29" s="29" t="s">
@@ -46770,7 +46769,7 @@
       <c r="K29">
         <v>7</v>
       </c>
-      <c r="L29" s="42" t="s">
+      <c r="L29" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M29" s="5" t="s">
@@ -46800,13 +46799,13 @@
       <c r="F30" t="s">
         <v>2715</v>
       </c>
-      <c r="G30" s="43">
+      <c r="G30" s="41">
         <v>333.57870000000003</v>
       </c>
       <c r="H30" t="s">
         <v>2715</v>
       </c>
-      <c r="I30" s="43">
+      <c r="I30" s="41">
         <v>1.1772</v>
       </c>
       <c r="J30" t="s">
@@ -46815,7 +46814,7 @@
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="L30" s="41" t="s">
+      <c r="L30" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M30" s="5" t="s">
@@ -46846,13 +46845,13 @@
       <c r="F31" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G31" s="43">
+      <c r="G31" s="41">
         <v>8.0732999999999997</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I31" s="43">
+      <c r="I31" s="41">
         <v>1.0102</v>
       </c>
       <c r="J31" s="29" t="s">
@@ -46861,7 +46860,7 @@
       <c r="K31">
         <v>1</v>
       </c>
-      <c r="L31" s="42" t="s">
+      <c r="L31" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M31" s="5" t="s">
@@ -46892,13 +46891,13 @@
       <c r="F32" t="s">
         <v>2715</v>
       </c>
-      <c r="G32" s="43">
+      <c r="G32" s="41">
         <v>8.8440820000000002</v>
       </c>
       <c r="H32" t="s">
         <v>2715</v>
       </c>
-      <c r="I32" s="43">
+      <c r="I32" s="41">
         <v>-51.503093</v>
       </c>
       <c r="J32" t="s">
@@ -46907,7 +46906,7 @@
       <c r="K32">
         <v>2</v>
       </c>
-      <c r="L32" s="41" t="s">
+      <c r="L32" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M32" s="6" t="s">
@@ -46938,13 +46937,13 @@
       <c r="F33" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G33" s="43">
+      <c r="G33" s="41">
         <v>332.24990000000003</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="41">
         <v>2.1152000000000002</v>
       </c>
       <c r="J33" s="29" t="s">
@@ -46953,7 +46952,7 @@
       <c r="K33">
         <v>1</v>
       </c>
-      <c r="L33" s="42" t="s">
+      <c r="L33" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M33" s="5" t="s">
@@ -46984,13 +46983,13 @@
       <c r="F34" t="s">
         <v>2715</v>
       </c>
-      <c r="G34" s="43">
+      <c r="G34" s="41">
         <v>37.700600000000001</v>
       </c>
       <c r="H34" t="s">
         <v>2715</v>
       </c>
-      <c r="I34" s="43">
+      <c r="I34" s="41">
         <v>-1.9841</v>
       </c>
       <c r="J34" t="s">
@@ -46999,7 +46998,7 @@
       <c r="K34">
         <v>1</v>
       </c>
-      <c r="L34" s="41" t="s">
+      <c r="L34" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M34" s="5" t="s">
@@ -47030,13 +47029,13 @@
       <c r="F35" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G35" s="43">
+      <c r="G35" s="41">
         <v>35.179625000000001</v>
       </c>
       <c r="H35" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I35" s="43">
+      <c r="I35" s="41">
         <v>-10.871236111111111</v>
       </c>
       <c r="J35" s="29" t="s">
@@ -47045,7 +47044,7 @@
       <c r="K35">
         <v>6</v>
       </c>
-      <c r="L35" s="42" t="s">
+      <c r="L35" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M35" s="5" t="s">
@@ -47076,13 +47075,13 @@
       <c r="F36" t="s">
         <v>2715</v>
       </c>
-      <c r="G36" s="43">
+      <c r="G36" s="41">
         <v>16.788599999999999</v>
       </c>
       <c r="H36" t="s">
         <v>2715</v>
       </c>
-      <c r="I36" s="43">
+      <c r="I36" s="41">
         <v>1.2918000000000001</v>
       </c>
       <c r="J36" t="s">
@@ -47091,7 +47090,7 @@
       <c r="K36">
         <v>1</v>
       </c>
-      <c r="L36" s="41" t="s">
+      <c r="L36" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M36" s="5" t="s">
@@ -47122,13 +47121,13 @@
       <c r="F37" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G37" s="43">
+      <c r="G37" s="41">
         <v>27.5379</v>
       </c>
       <c r="H37" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="41">
         <v>-3.0773000000000001</v>
       </c>
       <c r="J37" s="29" t="s">
@@ -47137,7 +47136,7 @@
       <c r="K37">
         <v>5</v>
       </c>
-      <c r="L37" s="42" t="s">
+      <c r="L37" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M37" s="7" t="s">
@@ -47168,13 +47167,13 @@
       <c r="F38" t="s">
         <v>2715</v>
       </c>
-      <c r="G38" s="43">
+      <c r="G38" s="41">
         <v>29.909300000000002</v>
       </c>
       <c r="H38" t="s">
         <v>2715</v>
       </c>
-      <c r="I38" s="43">
+      <c r="I38" s="41">
         <v>-3.9828999999999999</v>
       </c>
       <c r="J38" t="s">
@@ -47183,7 +47182,7 @@
       <c r="K38">
         <v>1</v>
       </c>
-      <c r="L38" s="41" t="s">
+      <c r="L38" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M38" s="5" t="s">
@@ -47214,13 +47213,13 @@
       <c r="F39" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G39" s="43">
+      <c r="G39" s="41">
         <v>7.7706999999999997</v>
       </c>
       <c r="H39" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I39" s="43">
+      <c r="I39" s="41">
         <v>-44.049100000000003</v>
       </c>
       <c r="J39" s="29" t="s">
@@ -47229,7 +47228,7 @@
       <c r="K39">
         <v>2</v>
       </c>
-      <c r="L39" s="42" t="s">
+      <c r="L39" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M39" s="5" t="s">
@@ -47260,13 +47259,13 @@
       <c r="F40" t="s">
         <v>2715</v>
       </c>
-      <c r="G40" s="43">
+      <c r="G40" s="41">
         <v>2.969506</v>
       </c>
       <c r="H40" t="s">
         <v>2715</v>
       </c>
-      <c r="I40" s="43">
+      <c r="I40" s="41">
         <v>-46.238942000000002</v>
       </c>
       <c r="J40" t="s">
@@ -47275,7 +47274,7 @@
       <c r="K40">
         <v>2</v>
       </c>
-      <c r="L40" s="41" t="s">
+      <c r="L40" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M40" s="6" t="s">
@@ -47306,13 +47305,13 @@
       <c r="F41" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G41" s="43">
+      <c r="G41" s="41">
         <v>2.068835</v>
       </c>
       <c r="H41" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I41" s="43">
+      <c r="I41" s="41">
         <v>-55.065944000000002</v>
       </c>
       <c r="J41" s="29" t="s">
@@ -47321,7 +47320,7 @@
       <c r="K41">
         <v>2</v>
       </c>
-      <c r="L41" s="42" t="s">
+      <c r="L41" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M41" s="5" t="s">
@@ -47352,13 +47351,13 @@
       <c r="F42" t="s">
         <v>2715</v>
       </c>
-      <c r="G42" s="43">
+      <c r="G42" s="41">
         <v>27.5379</v>
       </c>
       <c r="H42" t="s">
         <v>2715</v>
       </c>
-      <c r="I42" s="43">
+      <c r="I42" s="41">
         <v>-3.0773000000000001</v>
       </c>
       <c r="J42" t="s">
@@ -47367,7 +47366,7 @@
       <c r="K42">
         <v>5</v>
       </c>
-      <c r="L42" s="41" t="s">
+      <c r="L42" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M42" s="7" t="s">
@@ -47398,13 +47397,13 @@
       <c r="F43" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G43" s="43">
+      <c r="G43" s="41">
         <v>36.246875000000003</v>
       </c>
       <c r="H43" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I43" s="43">
+      <c r="I43" s="41">
         <v>-4.0177138888888893</v>
       </c>
       <c r="J43" s="29" t="s">
@@ -47413,7 +47412,7 @@
       <c r="K43">
         <v>6</v>
       </c>
-      <c r="L43" s="42" t="s">
+      <c r="L43" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M43" s="5" t="s">
@@ -47444,13 +47443,13 @@
       <c r="F44" t="s">
         <v>2715</v>
       </c>
-      <c r="G44" s="43">
+      <c r="G44" s="41">
         <v>36.246899999999997</v>
       </c>
       <c r="H44" t="s">
         <v>2715</v>
       </c>
-      <c r="I44" s="43">
+      <c r="I44" s="41">
         <v>-4.0176999999999996</v>
       </c>
       <c r="J44" t="s">
@@ -47459,7 +47458,7 @@
       <c r="K44">
         <v>3</v>
       </c>
-      <c r="L44" s="41" t="s">
+      <c r="L44" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M44" s="5" t="s">
@@ -47490,13 +47489,13 @@
       <c r="F45" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G45" s="43">
+      <c r="G45" s="41">
         <v>37.666499999999999</v>
       </c>
       <c r="H45" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I45" s="43">
+      <c r="I45" s="41">
         <v>-3.8411277777777779</v>
       </c>
       <c r="J45" s="29" t="s">
@@ -47505,7 +47504,7 @@
       <c r="K45">
         <v>6</v>
       </c>
-      <c r="L45" s="42" t="s">
+      <c r="L45" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M45" s="5" t="s">
@@ -47536,13 +47535,13 @@
       <c r="F46" t="s">
         <v>2715</v>
       </c>
-      <c r="G46" s="43">
+      <c r="G46" s="41">
         <v>3.7256999999999998</v>
       </c>
       <c r="H46" t="s">
         <v>2715</v>
       </c>
-      <c r="I46" s="43">
+      <c r="I46" s="41">
         <v>-0.95250000000000001</v>
       </c>
       <c r="J46" t="s">
@@ -47551,7 +47550,7 @@
       <c r="K46">
         <v>1</v>
       </c>
-      <c r="L46" s="41" t="s">
+      <c r="L46" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M46" s="5" t="s">
@@ -47582,13 +47581,13 @@
       <c r="F47" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="G47" s="43">
+      <c r="G47" s="41">
         <v>8.8440359999999991</v>
       </c>
       <c r="H47" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I47" s="43">
+      <c r="I47" s="41">
         <v>-51.509864</v>
       </c>
       <c r="J47" s="29" t="s">
@@ -47597,7 +47596,7 @@
       <c r="K47">
         <v>2</v>
       </c>
-      <c r="L47" s="42" t="s">
+      <c r="L47" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M47" s="5" t="s">
@@ -47628,13 +47627,13 @@
       <c r="F48" t="s">
         <v>2715</v>
       </c>
-      <c r="G48" s="43">
+      <c r="G48" s="41">
         <v>34.414833333333334</v>
       </c>
       <c r="H48" t="s">
         <v>2715</v>
       </c>
-      <c r="I48" s="43">
+      <c r="I48" s="41">
         <v>-10.555536111111111</v>
       </c>
       <c r="J48" t="s">
@@ -47643,7 +47642,7 @@
       <c r="K48">
         <v>6</v>
       </c>
-      <c r="L48" s="41" t="s">
+      <c r="L48" s="39" t="s">
         <v>2951</v>
       </c>
       <c r="M48" s="5" t="s">
@@ -47674,13 +47673,13 @@
       <c r="F49" s="23" t="s">
         <v>2715</v>
       </c>
-      <c r="G49" s="43">
+      <c r="G49" s="41">
         <v>338.04660000000001</v>
       </c>
       <c r="H49" s="23" t="s">
         <v>2715</v>
       </c>
-      <c r="I49" s="43">
+      <c r="I49" s="41">
         <v>0.95009999999999994</v>
       </c>
       <c r="J49" s="23" t="s">
@@ -47689,7 +47688,7 @@
       <c r="K49">
         <v>1</v>
       </c>
-      <c r="L49" s="42" t="s">
+      <c r="L49" s="40" t="s">
         <v>2951</v>
       </c>
       <c r="M49" s="5" t="s">
@@ -47761,56 +47760,6 @@
       <c r="R54" s="34"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{D168845F-828A-7347-9309-F35DE6E073A2}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{9C865400-E8B7-0249-9CD6-BCC9DABD81A0}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{A65B0BF3-26E0-A040-BC08-689006A371F9}"/>
-    <hyperlink ref="L6" r:id="rId4" xr:uid="{85683AF5-A00F-B349-BD13-9CFA393E783D}"/>
-    <hyperlink ref="L8" r:id="rId5" xr:uid="{700A2874-000F-DF41-B341-84742608A14F}"/>
-    <hyperlink ref="L10" r:id="rId6" xr:uid="{BEF99545-50C7-EA46-A495-3FFD1F4F4E7E}"/>
-    <hyperlink ref="L12" r:id="rId7" xr:uid="{36C5AA8A-BBF4-0945-8A25-F66DF0FEE9A6}"/>
-    <hyperlink ref="L14" r:id="rId8" xr:uid="{1622C234-171D-AF4E-962F-39CC79C46930}"/>
-    <hyperlink ref="L16" r:id="rId9" xr:uid="{607A881C-D91E-7847-975B-FB642D1CCCC5}"/>
-    <hyperlink ref="L18" r:id="rId10" xr:uid="{53E8F2DA-C665-994E-AF40-760A1E475B58}"/>
-    <hyperlink ref="L20" r:id="rId11" xr:uid="{50FD4E03-26CA-7848-A7F2-4FCA6CAAD194}"/>
-    <hyperlink ref="L22" r:id="rId12" xr:uid="{6776237B-4BE4-8A4F-8528-4645AC6FE680}"/>
-    <hyperlink ref="L24" r:id="rId13" xr:uid="{7F21D701-BBC1-0E45-AA01-E4FD799D2095}"/>
-    <hyperlink ref="L26" r:id="rId14" xr:uid="{FF8A417C-7A67-B34A-9D96-75491814BBEF}"/>
-    <hyperlink ref="L28" r:id="rId15" xr:uid="{9B759695-2AE9-8449-A21C-033B46855474}"/>
-    <hyperlink ref="L30" r:id="rId16" xr:uid="{5FC66173-E233-7643-8119-F43273340F04}"/>
-    <hyperlink ref="L32" r:id="rId17" xr:uid="{8FC44989-913D-4A4C-ACE4-E1266C098162}"/>
-    <hyperlink ref="L34" r:id="rId18" xr:uid="{395DDC2D-2930-AB4A-9B2E-09B3EE6A2DFE}"/>
-    <hyperlink ref="L36" r:id="rId19" xr:uid="{95106B88-F300-FD46-AFBA-AE2430FF2A11}"/>
-    <hyperlink ref="L38" r:id="rId20" xr:uid="{619FF774-43AC-3946-80AD-88A3C38CDEAE}"/>
-    <hyperlink ref="L40" r:id="rId21" xr:uid="{2DA8B9D1-5E17-2349-B908-053443D97BC7}"/>
-    <hyperlink ref="L42" r:id="rId22" xr:uid="{893E88E6-0C92-2649-A411-DCB734F36224}"/>
-    <hyperlink ref="L44" r:id="rId23" xr:uid="{A2505016-5A25-4F4D-BB3D-5931FF9AE816}"/>
-    <hyperlink ref="L46" r:id="rId24" xr:uid="{AB223FA8-5807-6743-9CDE-F962FE008809}"/>
-    <hyperlink ref="L48" r:id="rId25" xr:uid="{58133F4B-3D7E-D748-BFC3-B24EC2220930}"/>
-    <hyperlink ref="L5" r:id="rId26" xr:uid="{EDEB6FCA-4949-3549-A968-C9D087C4775C}"/>
-    <hyperlink ref="L7" r:id="rId27" xr:uid="{22796ACA-3CAD-E14A-AAC7-9EFFC06EFADF}"/>
-    <hyperlink ref="L9" r:id="rId28" xr:uid="{08F1E273-18E7-3F45-8D76-9F53136724DF}"/>
-    <hyperlink ref="L11" r:id="rId29" xr:uid="{800B7F12-656A-EC45-98EC-C7CFBC3999FD}"/>
-    <hyperlink ref="L13" r:id="rId30" xr:uid="{5267004C-DD01-F143-B706-D8A6E9727429}"/>
-    <hyperlink ref="L15" r:id="rId31" xr:uid="{193C1D44-B9BF-1D44-8865-79B75D5B7280}"/>
-    <hyperlink ref="L17" r:id="rId32" xr:uid="{2B74A97B-BAE6-804C-B746-B7AD389E37E9}"/>
-    <hyperlink ref="L19" r:id="rId33" xr:uid="{4995ADD4-E924-3446-9B6E-049BF1307A0F}"/>
-    <hyperlink ref="L21" r:id="rId34" xr:uid="{291179ED-47D9-784E-9076-CE06201FD4B8}"/>
-    <hyperlink ref="L23" r:id="rId35" xr:uid="{F1F48A4A-8021-1840-80A5-62CED52BB128}"/>
-    <hyperlink ref="L25" r:id="rId36" xr:uid="{4EBA3212-8951-4449-962E-78001EE8185B}"/>
-    <hyperlink ref="L27" r:id="rId37" xr:uid="{291EAA25-B1B4-B841-A9B6-2347B9BD33D2}"/>
-    <hyperlink ref="L29" r:id="rId38" xr:uid="{3DDA30EF-DCD4-3E46-BE02-85FC2994620E}"/>
-    <hyperlink ref="L31" r:id="rId39" xr:uid="{DE5CF654-30C2-6E4F-A6D1-668C239956B0}"/>
-    <hyperlink ref="L33" r:id="rId40" xr:uid="{4896E438-7D8C-6B44-9DE1-B395C290B446}"/>
-    <hyperlink ref="L35" r:id="rId41" xr:uid="{1542962A-667A-8E45-93FC-907D31D88964}"/>
-    <hyperlink ref="L37" r:id="rId42" xr:uid="{5B4BD416-25FF-2643-A95A-2DA4B1816DE7}"/>
-    <hyperlink ref="L39" r:id="rId43" xr:uid="{0B3B4823-B78E-C745-913B-59D2B8EB20B7}"/>
-    <hyperlink ref="L41" r:id="rId44" xr:uid="{20529E1E-3C47-4E44-81BF-E1C14F6EF5AE}"/>
-    <hyperlink ref="L43" r:id="rId45" xr:uid="{CE4CD744-ECEB-0C42-9DEB-12C1F529BE45}"/>
-    <hyperlink ref="L45" r:id="rId46" xr:uid="{E920F410-8A78-F640-B924-3C2708CE82BD}"/>
-    <hyperlink ref="L47" r:id="rId47" xr:uid="{1A9F08B7-6443-5F4D-BEA5-734DF9A41023}"/>
-    <hyperlink ref="L49" r:id="rId48" xr:uid="{4E4BB3AF-2FB6-6E4F-871B-E70618519185}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -53155,16 +53104,16 @@
       <c r="A1" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="42" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42" t="s">
         <v>1108</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="H1" t="s">
         <v>2357</v>
       </c>
@@ -64060,16 +64009,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">

</xml_diff>

<commit_message>
Trying to get magnitudes for found lenses
</commit_message>
<xml_diff>
--- a/Training/UnseenData/Unseen_KnownLenses.xlsx
+++ b/Training/UnseenData/Unseen_KnownLenses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Training/UnseenData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C634BFDF-5659-2646-8CEA-A362696FD8CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C7A4C9-AB3F-E74F-8C88-B35537C1E199}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
+    <workbookView xWindow="-35500" yWindow="-880" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{84A4477D-F980-D848-8C06-BB24D37B215E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lenses" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9403" uniqueCount="2997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9500" uniqueCount="3041">
   <si>
     <t>PAPER_TILE</t>
   </si>
@@ -9038,6 +9038,138 @@
   </si>
   <si>
     <t>Found in all 5</t>
+  </si>
+  <si>
+    <t>333.578416666667</t>
+  </si>
+  <si>
+    <t>33.3521666666667</t>
+  </si>
+  <si>
+    <t>33.533625</t>
+  </si>
+  <si>
+    <t>340.999</t>
+  </si>
+  <si>
+    <t>340.504916666667</t>
+  </si>
+  <si>
+    <t>14.7039583333333</t>
+  </si>
+  <si>
+    <t>35.826375</t>
+  </si>
+  <si>
+    <t>35.179625</t>
+  </si>
+  <si>
+    <t>36.246875</t>
+  </si>
+  <si>
+    <t>37.6665</t>
+  </si>
+  <si>
+    <t>34.4148333333333</t>
+  </si>
+  <si>
+    <t>-7.36575</t>
+  </si>
+  <si>
+    <t>-46.241202</t>
+  </si>
+  <si>
+    <t>1.17606944444444</t>
+  </si>
+  <si>
+    <t>-49.3903</t>
+  </si>
+  <si>
+    <t>-51.506618</t>
+  </si>
+  <si>
+    <t>-7.73189444444444</t>
+  </si>
+  <si>
+    <t>-41.555939</t>
+  </si>
+  <si>
+    <t>-40.6679</t>
+  </si>
+  <si>
+    <t>-46.238663</t>
+  </si>
+  <si>
+    <t>-3.7299</t>
+  </si>
+  <si>
+    <t>-0.3264</t>
+  </si>
+  <si>
+    <t>-5.59233055555555</t>
+  </si>
+  <si>
+    <t>-0.0803</t>
+  </si>
+  <si>
+    <t>-49.391714</t>
+  </si>
+  <si>
+    <t>2.46961388888889</t>
+  </si>
+  <si>
+    <t>-46.239201</t>
+  </si>
+  <si>
+    <t>-42.139283</t>
+  </si>
+  <si>
+    <t>-10.9801277777778</t>
+  </si>
+  <si>
+    <t>-3.6015</t>
+  </si>
+  <si>
+    <t>2.41527777777778</t>
+  </si>
+  <si>
+    <t>-51.503093</t>
+  </si>
+  <si>
+    <t>-1.9841</t>
+  </si>
+  <si>
+    <t>-10.8712361111111</t>
+  </si>
+  <si>
+    <t>-3.9829</t>
+  </si>
+  <si>
+    <t>-44.0491</t>
+  </si>
+  <si>
+    <t>-46.238942</t>
+  </si>
+  <si>
+    <t>-55.065944</t>
+  </si>
+  <si>
+    <t>-4.01771388888889</t>
+  </si>
+  <si>
+    <t>-4.0177</t>
+  </si>
+  <si>
+    <t>-3.84112777777778</t>
+  </si>
+  <si>
+    <t>-0.9525</t>
+  </si>
+  <si>
+    <t>-51.509864</t>
+  </si>
+  <si>
+    <t>-10.5555361111111</t>
   </si>
 </sst>
 </file>
@@ -48555,10 +48687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995C866F-3E57-F14D-B8B2-62FE8466E620}">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48569,15 +48701,15 @@
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.83203125" customWidth="1"/>
-    <col min="15" max="18" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="16.83203125" customWidth="1"/>
+    <col min="17" max="20" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="C1" s="36" t="s">
         <v>717</v>
       </c>
@@ -48593,42 +48725,48 @@
       <c r="G1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K1" s="28" t="s">
-        <v>2864</v>
-      </c>
-      <c r="L1" s="28"/>
       <c r="M1" s="28" t="s">
         <v>2864</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28" t="s">
+        <v>2864</v>
+      </c>
+      <c r="P1" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>2947</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>2946</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>2945</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>2948</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>2996</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>2895</v>
       </c>
@@ -48647,40 +48785,46 @@
       <c r="G2" s="41">
         <v>14.70392</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="41" t="s">
+        <v>2891</v>
+      </c>
+      <c r="I2" t="s">
         <v>2715</v>
       </c>
-      <c r="I2" s="41">
+      <c r="J2" s="41">
         <v>-7.3657500000000002</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="41" t="s">
+        <v>3008</v>
+      </c>
+      <c r="L2" t="s">
         <v>2715</v>
       </c>
-      <c r="K2" s="30">
+      <c r="M2" s="30">
         <v>4</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="N2" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>2848</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>2715</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>2896</v>
       </c>
-      <c r="R2" s="34" t="s">
+      <c r="T2" s="34" t="s">
         <v>2907</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="36" t="s">
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="36" t="s">
         <v>2995</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>2896</v>
       </c>
@@ -48699,40 +48843,46 @@
       <c r="G3" s="41">
         <v>33.288600000000002</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="41" t="s">
+        <v>876</v>
+      </c>
+      <c r="I3" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I3" s="41">
+      <c r="J3" s="41">
         <v>-24.229199999999999</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="K3" s="41" t="s">
+        <v>877</v>
+      </c>
+      <c r="L3" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>5</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="N3" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>1097</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="P3" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="S3" s="34" t="s">
         <v>2926</v>
-      </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34" t="s">
-        <v>2918</v>
       </c>
       <c r="T3" s="34"/>
       <c r="U3" s="34" t="s">
+        <v>2918</v>
+      </c>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34" t="s">
         <v>2901</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>2897</v>
       </c>
@@ -48751,38 +48901,44 @@
       <c r="G4" s="41">
         <v>2.9728940000000001</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
         <v>2715</v>
       </c>
-      <c r="I4" s="41">
+      <c r="J4" s="41">
         <v>-46.241202000000001</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="41" t="s">
+        <v>3009</v>
+      </c>
+      <c r="L4" t="s">
         <v>2715</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="N4" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>2715</v>
       </c>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
       <c r="S4" s="34"/>
-      <c r="T4" s="34" t="s">
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34" t="s">
         <v>2899</v>
       </c>
-      <c r="U4" s="34" t="s">
+      <c r="W4" s="34" t="s">
         <v>2910</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>2898</v>
       </c>
@@ -48801,38 +48957,44 @@
       <c r="G5" s="41">
         <v>333.57841666666701</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="41" t="s">
+        <v>2997</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I5" s="41">
+      <c r="J5" s="41">
         <v>1.1760694444444399</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="41" t="s">
+        <v>3010</v>
+      </c>
+      <c r="L5" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K5" s="30">
+      <c r="M5" s="30">
         <v>6</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="N5" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N5" s="29" t="s">
+      <c r="P5" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q5" s="34" t="s">
+      <c r="S5" s="34" t="s">
         <v>2930</v>
       </c>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
       <c r="T5" s="34"/>
-      <c r="U5" s="34" t="s">
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34" t="s">
         <v>2900</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>2899</v>
       </c>
@@ -48851,42 +49013,48 @@
       <c r="G6" s="41">
         <v>346.74279999999999</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="I6" t="s">
         <v>2715</v>
       </c>
-      <c r="I6" s="41">
+      <c r="J6" s="41">
         <v>2.4285999999999999</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="L6" t="s">
         <v>2715</v>
       </c>
-      <c r="K6" s="12">
-        <v>1</v>
-      </c>
-      <c r="L6" s="39" t="s">
+      <c r="M6" s="12">
+        <v>1</v>
+      </c>
+      <c r="N6" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>2715</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="S6" s="34" t="s">
         <v>2932</v>
       </c>
-      <c r="R6" s="34" t="s">
+      <c r="T6" s="34" t="s">
         <v>2923</v>
       </c>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34" t="s">
+      <c r="U6" s="34"/>
+      <c r="V6" s="34" t="s">
         <v>2921</v>
       </c>
-      <c r="U6" s="34" t="s">
+      <c r="W6" s="34" t="s">
         <v>2908</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>2900</v>
       </c>
@@ -48905,40 +49073,46 @@
       <c r="G7" s="41">
         <v>349.9726</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="41" t="s">
+        <v>2114</v>
+      </c>
+      <c r="I7" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I7" s="41">
+      <c r="J7" s="41">
         <v>0.63690000000000002</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="K7" s="41" t="s">
+        <v>2115</v>
+      </c>
+      <c r="L7" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K7" s="30">
-        <v>1</v>
-      </c>
-      <c r="L7" s="40" t="s">
+      <c r="M7" s="30">
+        <v>1</v>
+      </c>
+      <c r="N7" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="P7" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q7" s="34" t="s">
+      <c r="S7" s="34" t="s">
         <v>2933</v>
       </c>
-      <c r="R7" s="34" t="s">
+      <c r="T7" s="34" t="s">
         <v>2928</v>
       </c>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34" t="s">
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34" t="s">
         <v>2906</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>2901</v>
       </c>
@@ -48957,40 +49131,46 @@
       <c r="G8" s="41">
         <v>5.9326999999999996</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" t="s">
         <v>2715</v>
       </c>
-      <c r="I8" s="41">
+      <c r="J8" s="41">
         <v>-49.390300000000003</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" s="41" t="s">
+        <v>3011</v>
+      </c>
+      <c r="L8" t="s">
         <v>2715</v>
       </c>
-      <c r="K8" s="30">
+      <c r="M8" s="30">
         <v>2</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="N8" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>2715</v>
       </c>
-      <c r="Q8" s="34" t="s">
+      <c r="S8" s="34" t="s">
         <v>2934</v>
       </c>
-      <c r="R8" s="34" t="s">
+      <c r="T8" s="34" t="s">
         <v>2931</v>
       </c>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34" t="s">
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34" t="s">
         <v>2912</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>2902</v>
       </c>
@@ -49009,42 +49189,48 @@
       <c r="G9" s="41">
         <v>8.8458400000000008</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="41" t="s">
+        <v>2890</v>
+      </c>
+      <c r="I9" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I9" s="41">
+      <c r="J9" s="41">
         <v>-51.506618000000003</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="K9" s="41" t="s">
+        <v>3012</v>
+      </c>
+      <c r="L9" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K9" s="30">
+      <c r="M9" s="30">
         <v>2</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="N9" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="O9" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="P9" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="S9" s="34" t="s">
         <v>2936</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34" t="s">
+      <c r="T9" s="34"/>
+      <c r="U9" s="34" t="s">
         <v>2935</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="V9" s="34" t="s">
         <v>2905</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="W9" s="34" t="s">
         <v>2914</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>2903</v>
       </c>
@@ -49063,40 +49249,46 @@
       <c r="G10" s="41">
         <v>48.405999999999999</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="41" t="s">
+        <v>2886</v>
+      </c>
+      <c r="I10" t="s">
         <v>2715</v>
       </c>
-      <c r="I10" s="41">
+      <c r="J10" s="41">
         <v>-36.177700000000002</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" s="41" t="s">
+        <v>892</v>
+      </c>
+      <c r="L10" t="s">
         <v>2715</v>
       </c>
-      <c r="K10" s="30">
+      <c r="M10" s="30">
         <v>5</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="N10" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="O10" s="7" t="s">
         <v>1097</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>2715</v>
       </c>
-      <c r="Q10" s="34" t="s">
+      <c r="S10" s="34" t="s">
         <v>2937</v>
       </c>
-      <c r="R10" s="34" t="s">
+      <c r="T10" s="34" t="s">
         <v>2929</v>
       </c>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34" t="s">
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34" t="s">
         <v>2913</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>2904</v>
       </c>
@@ -49115,42 +49307,48 @@
       <c r="G11" s="41">
         <v>33.352166666666697</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="41" t="s">
+        <v>2998</v>
+      </c>
+      <c r="I11" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I11" s="41">
+      <c r="J11" s="41">
         <v>-7.7318944444444444</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="K11" s="41" t="s">
+        <v>3013</v>
+      </c>
+      <c r="L11" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K11" s="35">
+      <c r="M11" s="35">
         <v>6</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="N11" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="P11" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="S11" s="34" t="s">
         <v>2938</v>
       </c>
-      <c r="R11" s="34" t="s">
+      <c r="T11" s="34" t="s">
         <v>2944</v>
       </c>
-      <c r="S11" s="34" t="s">
+      <c r="U11" s="34" t="s">
         <v>2911</v>
       </c>
-      <c r="T11" s="34"/>
-      <c r="U11" s="34" t="s">
+      <c r="V11" s="34"/>
+      <c r="W11" s="34" t="s">
         <v>2902</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>2905</v>
       </c>
@@ -49169,44 +49367,50 @@
       <c r="G12" s="41">
         <v>346.74279999999999</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="I12" t="s">
         <v>2715</v>
       </c>
-      <c r="I12" s="41">
+      <c r="J12" s="41">
         <v>2.4285999999999999</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="L12" t="s">
         <v>2715</v>
       </c>
-      <c r="K12" s="30">
+      <c r="M12" s="30">
         <v>3</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="N12" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>2715</v>
       </c>
-      <c r="Q12" s="34" t="s">
+      <c r="S12" s="34" t="s">
         <v>2939</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="T12" s="36" t="s">
         <v>2940</v>
       </c>
-      <c r="S12" s="34" t="s">
+      <c r="U12" s="34" t="s">
         <v>2920</v>
       </c>
-      <c r="T12" s="34" t="s">
+      <c r="V12" s="34" t="s">
         <v>2922</v>
       </c>
-      <c r="U12" s="34" t="s">
+      <c r="W12" s="34" t="s">
         <v>2903</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>2906</v>
       </c>
@@ -49225,40 +49429,46 @@
       <c r="G13" s="41">
         <v>6.4905910000000002</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I13" s="41">
+      <c r="J13" s="41">
         <v>-41.555939000000002</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="K13" s="41" t="s">
+        <v>3014</v>
+      </c>
+      <c r="L13" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>2</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="N13" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N13" s="29" t="s">
+      <c r="P13" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q13" s="34" t="s">
+      <c r="S13" s="34" t="s">
         <v>2941</v>
       </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34" t="s">
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34" t="s">
         <v>2895</v>
       </c>
-      <c r="U13" s="34" t="s">
+      <c r="W13" s="34" t="s">
         <v>2898</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>2907</v>
       </c>
@@ -49277,40 +49487,46 @@
       <c r="G14" s="41">
         <v>5.3912000000000004</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
         <v>2715</v>
       </c>
-      <c r="I14" s="41">
+      <c r="J14" s="41">
         <v>-40.667900000000003</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" s="41" t="s">
+        <v>3015</v>
+      </c>
+      <c r="L14" t="s">
         <v>2715</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>2</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="N14" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>2715</v>
       </c>
-      <c r="Q14" s="34" t="s">
+      <c r="S14" s="34" t="s">
         <v>2942</v>
       </c>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34" t="s">
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34" t="s">
         <v>2924</v>
       </c>
-      <c r="U14" s="34" t="s">
+      <c r="W14" s="34" t="s">
         <v>2897</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>2908</v>
       </c>
@@ -49329,37 +49545,43 @@
       <c r="G15" s="41">
         <v>2.9729830000000002</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I15" s="41">
+      <c r="J15" s="41">
         <v>-46.238663000000003</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="K15" s="41" t="s">
+        <v>3016</v>
+      </c>
+      <c r="L15" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K15" s="12">
+      <c r="M15" s="12">
         <v>2</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="N15" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N15" s="29" t="s">
+      <c r="P15" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q15" s="34" t="s">
+      <c r="S15" s="34" t="s">
         <v>2943</v>
       </c>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34" t="s">
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34" t="s">
         <v>2919</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>2909</v>
       </c>
@@ -49378,37 +49600,43 @@
       <c r="G16" s="41">
         <v>32.814999999999998</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="41" t="s">
+        <v>2887</v>
+      </c>
+      <c r="I16" t="s">
         <v>2715</v>
       </c>
-      <c r="I16" s="41">
+      <c r="J16" s="41">
         <v>-3.7299000000000002</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" s="41" t="s">
+        <v>3017</v>
+      </c>
+      <c r="L16" t="s">
         <v>2715</v>
       </c>
-      <c r="K16" s="12">
-        <v>1</v>
-      </c>
-      <c r="L16" s="39" t="s">
+      <c r="M16" s="12">
+        <v>1</v>
+      </c>
+      <c r="N16" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>2715</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>2991</v>
       </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34" t="s">
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34" t="s">
         <v>2915</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>2910</v>
       </c>
@@ -49427,37 +49655,43 @@
       <c r="G17" s="41">
         <v>338.3331</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="41" t="s">
+        <v>2052</v>
+      </c>
+      <c r="I17" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I17" s="41">
+      <c r="J17" s="41">
         <v>-0.32640000000000002</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="K17" s="41" t="s">
+        <v>3018</v>
+      </c>
+      <c r="L17" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K17" s="12">
-        <v>1</v>
-      </c>
-      <c r="L17" s="40" t="s">
+      <c r="M17" s="12">
+        <v>1</v>
+      </c>
+      <c r="N17" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="P17" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q17" s="36" t="s">
+      <c r="S17" s="36" t="s">
         <v>2994</v>
       </c>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34" t="s">
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="34" t="s">
         <v>2909</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>2911</v>
       </c>
@@ -49476,37 +49710,43 @@
       <c r="G18" s="41">
         <v>33.533625000000001</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="41" t="s">
+        <v>2999</v>
+      </c>
+      <c r="I18" t="s">
         <v>2715</v>
       </c>
-      <c r="I18" s="41">
+      <c r="J18" s="41">
         <v>-5.5923305555555549</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" s="41" t="s">
+        <v>3019</v>
+      </c>
+      <c r="L18" t="s">
         <v>2715</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>6</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="N18" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="O18" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>2715</v>
       </c>
-      <c r="Q18" s="36" t="s">
+      <c r="S18" s="36" t="s">
         <v>2990</v>
       </c>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34" t="s">
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34" t="s">
         <v>2904</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>2912</v>
       </c>
@@ -49525,37 +49765,43 @@
       <c r="G19" s="41">
         <v>340.99900000000002</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="41" t="s">
+        <v>3000</v>
+      </c>
+      <c r="I19" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I19" s="41">
+      <c r="J19" s="41">
         <v>-8.0299999999999996E-2</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="K19" s="41" t="s">
+        <v>3020</v>
+      </c>
+      <c r="L19" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19" s="40" t="s">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N19" s="29" t="s">
+      <c r="P19" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q19" s="36" t="s">
+      <c r="S19" s="36" t="s">
         <v>2993</v>
       </c>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="34" t="s">
+      <c r="T19" s="34"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="34" t="s">
         <v>2925</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>2913</v>
       </c>
@@ -49574,37 +49820,43 @@
       <c r="G20" s="41">
         <v>6.4905910000000002</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" t="s">
         <v>2715</v>
       </c>
-      <c r="I20" s="41">
+      <c r="J20" s="41">
         <v>-41.555939000000002</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" s="41" t="s">
+        <v>3014</v>
+      </c>
+      <c r="L20" t="s">
         <v>2715</v>
       </c>
-      <c r="K20" s="30">
+      <c r="M20" s="30">
         <v>2</v>
       </c>
-      <c r="L20" s="39" t="s">
+      <c r="N20" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="O20" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>2715</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
         <v>2989</v>
       </c>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="34"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="34" t="s">
         <v>2927</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>2914</v>
       </c>
@@ -49623,52 +49875,58 @@
       <c r="G21" s="41">
         <v>5.9334790000000002</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I21" s="41">
+      <c r="J21" s="41">
         <v>-49.391714</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="K21" s="41" t="s">
+        <v>3021</v>
+      </c>
+      <c r="L21" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K21" s="12">
+      <c r="M21" s="12">
         <v>2</v>
       </c>
-      <c r="L21" s="40" t="s">
+      <c r="N21" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N21" s="29" t="s">
+      <c r="P21" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="P21" s="38" t="s">
+      <c r="R21" s="38" t="s">
         <v>2949</v>
       </c>
-      <c r="Q21" s="37">
-        <f>COUNTA(Q2:Q20)</f>
+      <c r="S21" s="37">
+        <f>COUNTA(S2:S20)</f>
         <v>18</v>
       </c>
-      <c r="R21" s="37">
-        <f t="shared" ref="R21:T21" si="0">COUNTA(R2:R20)</f>
+      <c r="T21" s="37">
+        <f t="shared" ref="T21:V21" si="0">COUNTA(T2:T20)</f>
         <v>7</v>
       </c>
-      <c r="S21" s="37">
+      <c r="U21" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="T21" s="37">
+      <c r="V21" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="U21" s="37">
-        <f>COUNTA(U2:U20)</f>
+      <c r="W21" s="37">
+        <f>COUNTA(W2:W20)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>2915</v>
       </c>
@@ -49687,52 +49945,58 @@
       <c r="G22" s="41">
         <v>340.50491666666699</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="41" t="s">
+        <v>3001</v>
+      </c>
+      <c r="I22" t="s">
         <v>2715</v>
       </c>
-      <c r="I22" s="41">
+      <c r="J22" s="41">
         <v>2.4696138888888899</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" s="41" t="s">
+        <v>3022</v>
+      </c>
+      <c r="L22" t="s">
         <v>2715</v>
       </c>
-      <c r="K22" s="30">
+      <c r="M22" s="30">
         <v>8</v>
       </c>
-      <c r="L22" s="39" t="s">
+      <c r="N22" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>2715</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="R22" s="38" t="s">
         <v>2950</v>
-      </c>
-      <c r="Q22" s="37">
-        <f>(Q21/A56)*100</f>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="R22" s="37">
-        <f>(R21/A56)*100</f>
-        <v>12.962962962962962</v>
       </c>
       <c r="S22" s="37">
         <f>(S21/A56)*100</f>
-        <v>7.4074074074074066</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="T22" s="37">
         <f>(T21/A56)*100</f>
-        <v>22.222222222222221</v>
+        <v>12.962962962962962</v>
       </c>
       <c r="U22" s="37">
         <f>(U21/A56)*100</f>
+        <v>7.4074074074074066</v>
+      </c>
+      <c r="V22" s="37">
+        <f>(V21/A56)*100</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="W22" s="37">
+        <f>(W21/A56)*100</f>
         <v>24.074074074074073</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>2916</v>
       </c>
@@ -49751,33 +50015,39 @@
       <c r="G23" s="41">
         <v>2.9736099999999999</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="41" t="s">
+        <v>2893</v>
+      </c>
+      <c r="I23" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I23" s="41">
+      <c r="J23" s="41">
         <v>-46.239201000000001</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="K23" s="41" t="s">
+        <v>3023</v>
+      </c>
+      <c r="L23" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K23" s="12">
+      <c r="M23" s="12">
         <v>2</v>
       </c>
-      <c r="L23" s="40" t="s">
+      <c r="N23" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N23" s="29" t="s">
+      <c r="P23" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
       <c r="S23" s="34"/>
       <c r="T23" s="34"/>
-    </row>
-    <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
+    </row>
+    <row r="24" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>2917</v>
       </c>
@@ -49796,33 +50066,39 @@
       <c r="G24" s="41">
         <v>340.5899</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="41" t="s">
+        <v>692</v>
+      </c>
+      <c r="I24" t="s">
         <v>2715</v>
       </c>
-      <c r="I24" s="41">
+      <c r="J24" s="41">
         <v>0.1958</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" s="41" t="s">
+        <v>693</v>
+      </c>
+      <c r="L24" t="s">
         <v>2715</v>
       </c>
-      <c r="K24" s="12">
+      <c r="M24" s="12">
         <v>3</v>
       </c>
-      <c r="L24" s="39" t="s">
+      <c r="N24" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>2715</v>
       </c>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
       <c r="S24" s="34"/>
       <c r="T24" s="34"/>
-    </row>
-    <row r="25" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
+    </row>
+    <row r="25" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>2918</v>
       </c>
@@ -49841,33 +50117,39 @@
       <c r="G25" s="41">
         <v>1.512545</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I25" s="41">
+      <c r="J25" s="41">
         <v>-42.139282999999999</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="K25" s="41" t="s">
+        <v>3024</v>
+      </c>
+      <c r="L25" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K25" s="12">
+      <c r="M25" s="12">
         <v>2</v>
       </c>
-      <c r="L25" s="40" t="s">
+      <c r="N25" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="O25" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N25" s="29" t="s">
+      <c r="P25" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
       <c r="S25" s="34"/>
       <c r="T25" s="34"/>
-    </row>
-    <row r="26" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U25" s="34"/>
+      <c r="V25" s="34"/>
+    </row>
+    <row r="26" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>2919</v>
       </c>
@@ -49886,33 +50168,39 @@
       <c r="G26" s="41">
         <v>14.703958333333334</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="41" t="s">
+        <v>3002</v>
+      </c>
+      <c r="I26" t="s">
         <v>2715</v>
       </c>
-      <c r="I26" s="41">
+      <c r="J26" s="41">
         <v>-7.3657499999999994</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" s="41" t="s">
+        <v>3008</v>
+      </c>
+      <c r="L26" t="s">
         <v>2715</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>4</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="N26" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>2848</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>2715</v>
       </c>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
       <c r="S26" s="34"/>
       <c r="T26" s="34"/>
-    </row>
-    <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
+    </row>
+    <row r="27" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
         <v>2920</v>
       </c>
@@ -49931,33 +50219,39 @@
       <c r="G27" s="41">
         <v>35.826374999999999</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="41" t="s">
+        <v>3003</v>
+      </c>
+      <c r="I27" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I27" s="41">
+      <c r="J27" s="41">
         <v>-10.980127777777778</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="K27" s="41" t="s">
+        <v>3025</v>
+      </c>
+      <c r="L27" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>6</v>
       </c>
-      <c r="L27" s="40" t="s">
+      <c r="N27" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="O27" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="P27" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
       <c r="S27" s="34"/>
       <c r="T27" s="34"/>
-    </row>
-    <row r="28" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
+    </row>
+    <row r="28" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>2921</v>
       </c>
@@ -49976,33 +50270,39 @@
       <c r="G28" s="41">
         <v>36.043700000000001</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="41" t="s">
+        <v>1230</v>
+      </c>
+      <c r="I28" t="s">
         <v>2715</v>
       </c>
-      <c r="I28" s="41">
+      <c r="J28" s="41">
         <v>-3.6015000000000001</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" s="41" t="s">
+        <v>3026</v>
+      </c>
+      <c r="L28" t="s">
         <v>2715</v>
       </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" s="39" t="s">
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="O28" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>2715</v>
       </c>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
-    </row>
-    <row r="29" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
+    </row>
+    <row r="29" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
         <v>2922</v>
       </c>
@@ -50021,33 +50321,39 @@
       <c r="G29" s="41">
         <v>0</v>
       </c>
-      <c r="H29" s="29" t="s">
+      <c r="H29" s="41">
+        <v>0</v>
+      </c>
+      <c r="I29" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I29" s="41">
+      <c r="J29" s="41">
         <v>2.4152777777777779</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="K29" s="41" t="s">
+        <v>3027</v>
+      </c>
+      <c r="L29" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>7</v>
       </c>
-      <c r="L29" s="40" t="s">
+      <c r="N29" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="O29" s="5" t="s">
         <v>2356</v>
       </c>
-      <c r="N29" s="29" t="s">
+      <c r="P29" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
       <c r="S29" s="34"/>
       <c r="T29" s="34"/>
-    </row>
-    <row r="30" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+    </row>
+    <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>2923</v>
       </c>
@@ -50066,33 +50372,39 @@
       <c r="G30" s="41">
         <v>333.57870000000003</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="41" t="s">
+        <v>2003</v>
+      </c>
+      <c r="I30" t="s">
         <v>2715</v>
       </c>
-      <c r="I30" s="41">
+      <c r="J30" s="41">
         <v>1.1772</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" s="41" t="s">
+        <v>2004</v>
+      </c>
+      <c r="L30" t="s">
         <v>2715</v>
       </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30" s="39" t="s">
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="O30" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>2715</v>
       </c>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
       <c r="S30" s="34"/>
       <c r="T30" s="34"/>
-    </row>
-    <row r="31" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+    </row>
+    <row r="31" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>2925</v>
       </c>
@@ -50112,33 +50424,39 @@
       <c r="G31" s="41">
         <v>8.0732999999999997</v>
       </c>
-      <c r="H31" s="29" t="s">
+      <c r="H31" s="41" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I31" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I31" s="41">
+      <c r="J31" s="41">
         <v>1.0102</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="K31" s="41" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L31" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31" s="40" t="s">
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="O31" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N31" s="29" t="s">
+      <c r="P31" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="34"/>
       <c r="S31" s="34"/>
       <c r="T31" s="34"/>
-    </row>
-    <row r="32" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
+    </row>
+    <row r="32" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>2926</v>
       </c>
@@ -50158,33 +50476,39 @@
       <c r="G32" s="41">
         <v>8.8440820000000002</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" t="s">
         <v>2715</v>
       </c>
-      <c r="I32" s="41">
+      <c r="J32" s="41">
         <v>-51.503093</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" s="41" t="s">
+        <v>3028</v>
+      </c>
+      <c r="L32" t="s">
         <v>2715</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>2</v>
       </c>
-      <c r="L32" s="39" t="s">
+      <c r="N32" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="O32" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N32" t="s">
+      <c r="P32" t="s">
         <v>2715</v>
       </c>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
       <c r="S32" s="34"/>
       <c r="T32" s="34"/>
-    </row>
-    <row r="33" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+    </row>
+    <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>2928</v>
       </c>
@@ -50204,33 +50528,39 @@
       <c r="G33" s="41">
         <v>332.24990000000003</v>
       </c>
-      <c r="H33" s="29" t="s">
+      <c r="H33" s="41" t="s">
+        <v>1963</v>
+      </c>
+      <c r="I33" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I33" s="41">
+      <c r="J33" s="41">
         <v>2.1152000000000002</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="K33" s="41" t="s">
+        <v>1964</v>
+      </c>
+      <c r="L33" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" s="40" t="s">
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="O33" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N33" s="29" t="s">
+      <c r="P33" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
       <c r="S33" s="34"/>
       <c r="T33" s="34"/>
-    </row>
-    <row r="34" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+    </row>
+    <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>2929</v>
       </c>
@@ -50250,33 +50580,39 @@
       <c r="G34" s="41">
         <v>37.700600000000001</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="41" t="s">
+        <v>1247</v>
+      </c>
+      <c r="I34" t="s">
         <v>2715</v>
       </c>
-      <c r="I34" s="41">
+      <c r="J34" s="41">
         <v>-1.9841</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" s="41" t="s">
+        <v>3029</v>
+      </c>
+      <c r="L34" t="s">
         <v>2715</v>
       </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" s="39" t="s">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N34" t="s">
+      <c r="P34" t="s">
         <v>2715</v>
       </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
       <c r="S34" s="34"/>
       <c r="T34" s="34"/>
-    </row>
-    <row r="35" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+    </row>
+    <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>2930</v>
       </c>
@@ -50296,33 +50632,39 @@
       <c r="G35" s="41">
         <v>35.179625000000001</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H35" s="41" t="s">
+        <v>3004</v>
+      </c>
+      <c r="I35" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I35" s="41">
+      <c r="J35" s="41">
         <v>-10.871236111111111</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="K35" s="41" t="s">
+        <v>3030</v>
+      </c>
+      <c r="L35" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>6</v>
       </c>
-      <c r="L35" s="40" t="s">
+      <c r="N35" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="O35" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N35" s="29" t="s">
+      <c r="P35" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
       <c r="S35" s="34"/>
       <c r="T35" s="34"/>
-    </row>
-    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U35" s="34"/>
+      <c r="V35" s="34"/>
+    </row>
+    <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
         <v>2931</v>
       </c>
@@ -50342,33 +50684,39 @@
       <c r="G36" s="41">
         <v>16.788599999999999</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="41" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I36" t="s">
         <v>2715</v>
       </c>
-      <c r="I36" s="41">
+      <c r="J36" s="41">
         <v>1.2918000000000001</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" s="41" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L36" t="s">
         <v>2715</v>
       </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36" s="39" t="s">
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M36" s="5" t="s">
+      <c r="O36" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N36" t="s">
+      <c r="P36" t="s">
         <v>2715</v>
       </c>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
       <c r="S36" s="34"/>
       <c r="T36" s="34"/>
-    </row>
-    <row r="37" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
+    </row>
+    <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
         <v>2932</v>
       </c>
@@ -50388,33 +50736,39 @@
       <c r="G37" s="41">
         <v>27.5379</v>
       </c>
-      <c r="H37" s="29" t="s">
+      <c r="H37" s="41" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I37" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I37" s="41">
+      <c r="J37" s="41">
         <v>-3.0773000000000001</v>
       </c>
-      <c r="J37" s="29" t="s">
+      <c r="K37" s="41" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L37" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>5</v>
       </c>
-      <c r="L37" s="40" t="s">
+      <c r="N37" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="O37" s="7" t="s">
         <v>1097</v>
       </c>
-      <c r="N37" s="29" t="s">
+      <c r="P37" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
       <c r="S37" s="34"/>
       <c r="T37" s="34"/>
-    </row>
-    <row r="38" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+    </row>
+    <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
         <v>2933</v>
       </c>
@@ -50434,33 +50788,39 @@
       <c r="G38" s="41">
         <v>29.909300000000002</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="41" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I38" t="s">
         <v>2715</v>
       </c>
-      <c r="I38" s="41">
+      <c r="J38" s="41">
         <v>-3.9828999999999999</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" s="41" t="s">
+        <v>3031</v>
+      </c>
+      <c r="L38" t="s">
         <v>2715</v>
       </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38" s="39" t="s">
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M38" s="5" t="s">
+      <c r="O38" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N38" t="s">
+      <c r="P38" t="s">
         <v>2715</v>
       </c>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
       <c r="S38" s="34"/>
       <c r="T38" s="34"/>
-    </row>
-    <row r="39" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U38" s="34"/>
+      <c r="V38" s="34"/>
+    </row>
+    <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>2934</v>
       </c>
@@ -50480,33 +50840,39 @@
       <c r="G39" s="41">
         <v>7.7706999999999997</v>
       </c>
-      <c r="H39" s="29" t="s">
+      <c r="H39" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I39" s="41">
+      <c r="J39" s="41">
         <v>-44.049100000000003</v>
       </c>
-      <c r="J39" s="29" t="s">
+      <c r="K39" s="41" t="s">
+        <v>3032</v>
+      </c>
+      <c r="L39" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>2</v>
       </c>
-      <c r="L39" s="40" t="s">
+      <c r="N39" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="O39" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N39" s="29" t="s">
+      <c r="P39" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
       <c r="S39" s="34"/>
       <c r="T39" s="34"/>
-    </row>
-    <row r="40" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U39" s="34"/>
+      <c r="V39" s="34"/>
+    </row>
+    <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>2935</v>
       </c>
@@ -50526,33 +50892,39 @@
       <c r="G40" s="41">
         <v>2.969506</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" t="s">
         <v>2715</v>
       </c>
-      <c r="I40" s="41">
+      <c r="J40" s="41">
         <v>-46.238942000000002</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" s="41" t="s">
+        <v>3033</v>
+      </c>
+      <c r="L40" t="s">
         <v>2715</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>2</v>
       </c>
-      <c r="L40" s="39" t="s">
+      <c r="N40" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M40" s="6" t="s">
+      <c r="O40" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="N40" t="s">
+      <c r="P40" t="s">
         <v>2715</v>
       </c>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
       <c r="S40" s="34"/>
       <c r="T40" s="34"/>
-    </row>
-    <row r="41" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+    </row>
+    <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>2936</v>
       </c>
@@ -50572,33 +50944,39 @@
       <c r="G41" s="41">
         <v>2.068835</v>
       </c>
-      <c r="H41" s="29" t="s">
+      <c r="H41" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I41" s="41">
+      <c r="J41" s="41">
         <v>-55.065944000000002</v>
       </c>
-      <c r="J41" s="29" t="s">
+      <c r="K41" s="41" t="s">
+        <v>3034</v>
+      </c>
+      <c r="L41" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>2</v>
       </c>
-      <c r="L41" s="40" t="s">
+      <c r="N41" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="O41" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N41" s="29" t="s">
+      <c r="P41" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="34"/>
       <c r="S41" s="34"/>
       <c r="T41" s="34"/>
-    </row>
-    <row r="42" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+    </row>
+    <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>2937</v>
       </c>
@@ -50618,33 +50996,39 @@
       <c r="G42" s="41">
         <v>27.5379</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="41" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I42" t="s">
         <v>2715</v>
       </c>
-      <c r="I42" s="41">
+      <c r="J42" s="41">
         <v>-3.0773000000000001</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" s="41" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L42" t="s">
         <v>2715</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <v>5</v>
       </c>
-      <c r="L42" s="39" t="s">
+      <c r="N42" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M42" s="7" t="s">
+      <c r="O42" s="7" t="s">
         <v>1097</v>
       </c>
-      <c r="N42" t="s">
+      <c r="P42" t="s">
         <v>2715</v>
       </c>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="34"/>
       <c r="S42" s="34"/>
       <c r="T42" s="34"/>
-    </row>
-    <row r="43" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+    </row>
+    <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>2938</v>
       </c>
@@ -50664,33 +51048,39 @@
       <c r="G43" s="41">
         <v>36.246875000000003</v>
       </c>
-      <c r="H43" s="29" t="s">
+      <c r="H43" s="41" t="s">
+        <v>3005</v>
+      </c>
+      <c r="I43" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I43" s="41">
+      <c r="J43" s="41">
         <v>-4.0177138888888893</v>
       </c>
-      <c r="J43" s="29" t="s">
+      <c r="K43" s="41" t="s">
+        <v>3035</v>
+      </c>
+      <c r="L43" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>6</v>
       </c>
-      <c r="L43" s="40" t="s">
+      <c r="N43" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M43" s="5" t="s">
+      <c r="O43" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N43" s="29" t="s">
+      <c r="P43" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="34"/>
       <c r="S43" s="34"/>
       <c r="T43" s="34"/>
-    </row>
-    <row r="44" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U43" s="34"/>
+      <c r="V43" s="34"/>
+    </row>
+    <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>2939</v>
       </c>
@@ -50710,33 +51100,39 @@
       <c r="G44" s="41">
         <v>36.246899999999997</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="41" t="s">
+        <v>2522</v>
+      </c>
+      <c r="I44" t="s">
         <v>2715</v>
       </c>
-      <c r="I44" s="41">
+      <c r="J44" s="41">
         <v>-4.0176999999999996</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" s="41" t="s">
+        <v>3036</v>
+      </c>
+      <c r="L44" t="s">
         <v>2715</v>
       </c>
-      <c r="K44">
+      <c r="M44">
         <v>3</v>
       </c>
-      <c r="L44" s="39" t="s">
+      <c r="N44" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="O44" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="N44" t="s">
+      <c r="P44" t="s">
         <v>2715</v>
       </c>
-      <c r="Q44" s="34"/>
-      <c r="R44" s="34"/>
       <c r="S44" s="34"/>
       <c r="T44" s="34"/>
-    </row>
-    <row r="45" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U44" s="34"/>
+      <c r="V44" s="34"/>
+    </row>
+    <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="36" t="s">
         <v>2940</v>
       </c>
@@ -50756,33 +51152,39 @@
       <c r="G45" s="41">
         <v>37.666499999999999</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="41" t="s">
+        <v>3006</v>
+      </c>
+      <c r="I45" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I45" s="41">
+      <c r="J45" s="41">
         <v>-3.8411277777777779</v>
       </c>
-      <c r="J45" s="29" t="s">
+      <c r="K45" s="41" t="s">
+        <v>3037</v>
+      </c>
+      <c r="L45" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K45">
+      <c r="M45">
         <v>6</v>
       </c>
-      <c r="L45" s="40" t="s">
+      <c r="N45" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M45" s="5" t="s">
+      <c r="O45" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N45" s="29" t="s">
+      <c r="P45" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q45" s="34"/>
-      <c r="R45" s="34"/>
       <c r="S45" s="34"/>
       <c r="T45" s="34"/>
-    </row>
-    <row r="46" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+    </row>
+    <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="36" t="s">
         <v>2941</v>
       </c>
@@ -50802,33 +51204,39 @@
       <c r="G46" s="41">
         <v>3.7256999999999998</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="41" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I46" t="s">
         <v>2715</v>
       </c>
-      <c r="I46" s="41">
+      <c r="J46" s="41">
         <v>-0.95250000000000001</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" s="41" t="s">
+        <v>3038</v>
+      </c>
+      <c r="L46" t="s">
         <v>2715</v>
       </c>
-      <c r="K46">
-        <v>1</v>
-      </c>
-      <c r="L46" s="39" t="s">
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M46" s="5" t="s">
+      <c r="O46" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N46" t="s">
+      <c r="P46" t="s">
         <v>2715</v>
       </c>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
       <c r="S46" s="34"/>
       <c r="T46" s="34"/>
-    </row>
-    <row r="47" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U46" s="34"/>
+      <c r="V46" s="34"/>
+    </row>
+    <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="36" t="s">
         <v>2942</v>
       </c>
@@ -50848,33 +51256,39 @@
       <c r="G47" s="41">
         <v>8.8440359999999991</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="H47" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I47" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="I47" s="41">
+      <c r="J47" s="41">
         <v>-51.509864</v>
       </c>
-      <c r="J47" s="29" t="s">
+      <c r="K47" s="41" t="s">
+        <v>3039</v>
+      </c>
+      <c r="L47" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="K47">
+      <c r="M47">
         <v>2</v>
       </c>
-      <c r="L47" s="40" t="s">
+      <c r="N47" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="O47" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N47" s="29" t="s">
+      <c r="P47" s="29" t="s">
         <v>2715</v>
       </c>
-      <c r="Q47" s="34"/>
-      <c r="R47" s="34"/>
       <c r="S47" s="34"/>
       <c r="T47" s="34"/>
-    </row>
-    <row r="48" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U47" s="34"/>
+      <c r="V47" s="34"/>
+    </row>
+    <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="36" t="s">
         <v>2944</v>
       </c>
@@ -50894,33 +51308,39 @@
       <c r="G48" s="41">
         <v>34.414833333333334</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="41" t="s">
+        <v>3007</v>
+      </c>
+      <c r="I48" t="s">
         <v>2715</v>
       </c>
-      <c r="I48" s="41">
+      <c r="J48" s="41">
         <v>-10.555536111111111</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" s="41" t="s">
+        <v>3040</v>
+      </c>
+      <c r="L48" t="s">
         <v>2715</v>
       </c>
-      <c r="K48">
+      <c r="M48">
         <v>6</v>
       </c>
-      <c r="L48" s="39" t="s">
+      <c r="N48" s="39" t="s">
         <v>2951</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="O48" s="5" t="s">
         <v>2508</v>
       </c>
-      <c r="N48" t="s">
+      <c r="P48" t="s">
         <v>2715</v>
       </c>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
       <c r="S48" s="34"/>
       <c r="T48" s="34"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U48" s="34"/>
+      <c r="V48" s="34"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
         <v>2943</v>
       </c>
@@ -50940,33 +51360,39 @@
       <c r="G49" s="41">
         <v>338.04660000000001</v>
       </c>
-      <c r="H49" s="23" t="s">
+      <c r="H49" s="41" t="s">
+        <v>2041</v>
+      </c>
+      <c r="I49" s="23" t="s">
         <v>2715</v>
       </c>
-      <c r="I49" s="41">
+      <c r="J49" s="41">
         <v>0.95009999999999994</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="K49" s="41" t="s">
+        <v>2042</v>
+      </c>
+      <c r="L49" s="23" t="s">
         <v>2715</v>
       </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49" s="40" t="s">
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49" s="40" t="s">
         <v>2951</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="O49" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="N49" s="23" t="s">
+      <c r="P49" s="23" t="s">
         <v>2715</v>
       </c>
-      <c r="Q49" s="34"/>
-      <c r="R49" s="34"/>
       <c r="S49" s="34"/>
       <c r="T49" s="34"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U49" s="34"/>
+      <c r="V49" s="34"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>2994</v>
       </c>
@@ -50974,18 +51400,20 @@
       <c r="D50" s="23"/>
       <c r="F50" s="23"/>
       <c r="G50" s="41"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="23"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="23"/>
-      <c r="Q50" s="34"/>
-      <c r="R50" s="34"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="23"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="23"/>
       <c r="S50" s="34"/>
       <c r="T50" s="34"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U50" s="34"/>
+      <c r="V50" s="34"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>2990</v>
       </c>
@@ -50993,18 +51421,20 @@
       <c r="D51" s="23"/>
       <c r="F51" s="23"/>
       <c r="G51" s="41"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="23"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="23"/>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="34"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="23"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="23"/>
       <c r="S51" s="34"/>
       <c r="T51" s="34"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U51" s="34"/>
+      <c r="V51" s="34"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>2993</v>
       </c>
@@ -51012,18 +51442,20 @@
       <c r="D52" s="23"/>
       <c r="F52" s="23"/>
       <c r="G52" s="41"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="23"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="23"/>
-      <c r="Q52" s="34"/>
-      <c r="R52" s="34"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="23"/>
+      <c r="N52" s="40"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="23"/>
       <c r="S52" s="34"/>
       <c r="T52" s="34"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U52" s="34"/>
+      <c r="V52" s="34"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>2989</v>
       </c>
@@ -51031,18 +51463,20 @@
       <c r="D53" s="23"/>
       <c r="F53" s="23"/>
       <c r="G53" s="41"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="23"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="23"/>
-      <c r="Q53" s="34"/>
-      <c r="R53" s="34"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="23"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="23"/>
       <c r="S53" s="34"/>
       <c r="T53" s="34"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U53" s="34"/>
+      <c r="V53" s="34"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>2991</v>
       </c>
@@ -51050,18 +51484,20 @@
       <c r="D54" s="23"/>
       <c r="F54" s="23"/>
       <c r="G54" s="41"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="23"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="23"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="23"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="23"/>
       <c r="S54" s="34"/>
       <c r="T54" s="34"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U54" s="34"/>
+      <c r="V54" s="34"/>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>2992</v>
       </c>
@@ -51069,13 +51505,14 @@
       <c r="E55" s="29"/>
       <c r="F55" s="31"/>
       <c r="G55" s="5"/>
-      <c r="H55" s="12"/>
-      <c r="O55" s="34"/>
-      <c r="P55" s="34"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="12"/>
       <c r="Q55" s="34"/>
       <c r="R55" s="34"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S55" s="34"/>
+      <c r="T55" s="34"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="38">
         <f>COUNTA(A1:A55)</f>
         <v>54</v>
@@ -51089,37 +51526,41 @@
       <c r="E56" s="31"/>
       <c r="F56" s="31"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="30"/>
+      <c r="H56" s="6"/>
       <c r="I56" s="30"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="34"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
       <c r="P56" s="34"/>
       <c r="Q56" s="34"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R56" s="34"/>
+      <c r="S56" s="34"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D57" s="31"/>
       <c r="E57" s="29"/>
       <c r="F57" s="31"/>
       <c r="G57" s="31"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="12"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="5"/>
       <c r="J57" s="12"/>
-      <c r="O57" s="34"/>
-      <c r="P57" s="34"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
       <c r="Q57" s="34"/>
       <c r="R57" s="34"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="O58" s="34"/>
-      <c r="P58" s="34"/>
+      <c r="S57" s="34"/>
+      <c r="T57" s="34"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="Q58" s="34"/>
       <c r="R58" s="34"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
+      <c r="S58" s="34"/>
+      <c r="T58" s="34"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="Q59" s="34"/>
       <c r="R59" s="34"/>
+      <c r="S59" s="34"/>
+      <c r="T59" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51130,7 +51571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976FD3A7-3202-C743-846D-2E8ADD6ECC71}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -54144,7 +54585,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F27"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>